<commit_message>
Added result of all models for up to 32 processes
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -2,18 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toaxo\Desktop\MSU\Sem5\Hausdorff\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E66E3703-8961-4401-B91C-757A6A3F23A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9C21BC-A389-4BEA-8A06-CA585723A021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2AFDC7F-E8CC-4187-9F4B-7A735A4181DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B2AFDC7F-E8CC-4187-9F4B-7A735A4181DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="27">
   <si>
     <t>PROCESSES</t>
   </si>
@@ -45,15 +47,87 @@
   <si>
     <t>TIME (s)</t>
   </si>
+  <si>
+    <t>GoldenRetriever</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Horse</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Eagle</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
+  </si>
+  <si>
+    <t>Dolphin -&gt; M11</t>
+  </si>
+  <si>
+    <t>Bull</t>
+  </si>
+  <si>
+    <t>Bull -&gt; M8</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Dog -&gt; M1</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>Camel -&gt; M10</t>
+  </si>
+  <si>
+    <t>Giraffe</t>
+  </si>
+  <si>
+    <t>Giraffe -&gt; M9</t>
+  </si>
+  <si>
+    <t>Human -&gt; M3</t>
+  </si>
+  <si>
+    <t>GoldenRetriever -&gt; M8</t>
+  </si>
+  <si>
+    <t>Wolf -&gt; M1</t>
+  </si>
+  <si>
+    <t>Horse -&gt; M11</t>
+  </si>
+  <si>
+    <t>Lion -&gt; M2</t>
+  </si>
+  <si>
+    <t>Eagle -&gt; M2</t>
+  </si>
+  <si>
+    <t>Среднее Ускорение</t>
+  </si>
+  <si>
+    <t>Vertices</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,16 +145,167 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -103,20 +328,676 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="13" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,6 +1774,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1228600336"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1528,16 +2410,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>79513</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>123822</xdr:rowOff>
+      <xdr:rowOff>57978</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>414131</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>173933</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1864,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4FF6C2-EC25-4B3E-BCE0-855100FCA57B}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,6 +2840,9 @@
         <v>27.877063074107514</v>
       </c>
     </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+    </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S15" s="6"/>
     </row>
@@ -1966,4 +2851,2219 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70DCB3C-3F08-4ABF-81AB-DC0E48A72EC9}">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22:L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="30"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="21"/>
+      <c r="P2" s="22"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="16"/>
+      <c r="N3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6344.3038299999998</v>
+      </c>
+      <c r="C4" s="10">
+        <f>$B$4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6109.1739200000002</v>
+      </c>
+      <c r="E4" s="10">
+        <f>$D$4/D4</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="J4" s="8">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1238.5593100000001</v>
+      </c>
+      <c r="L4" s="10">
+        <f>$K$4/K4</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="8">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>3805.0702200000001</v>
+      </c>
+      <c r="P4" s="10">
+        <f>$O$4/O4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3211.6042600000001</v>
+      </c>
+      <c r="C5" s="10">
+        <f>$B$4/B5</f>
+        <v>1.9754313783355113</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3009.9733200000001</v>
+      </c>
+      <c r="E5" s="10">
+        <f>$D$4/D5</f>
+        <v>2.0296438773749661</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="J5" s="8">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>635.85972000000004</v>
+      </c>
+      <c r="L5" s="10">
+        <f>$K$4/K5</f>
+        <v>1.9478499282829238</v>
+      </c>
+      <c r="N5" s="8">
+        <v>2</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1904.85754</v>
+      </c>
+      <c r="P5" s="10">
+        <f>$O$4/O5</f>
+        <v>1.997561570929866</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1581.87771</v>
+      </c>
+      <c r="C6" s="10">
+        <f>$B$4/B6</f>
+        <v>4.0106158585419349</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1535.1008899999999</v>
+      </c>
+      <c r="E6" s="10">
+        <f>$D$4/D6</f>
+        <v>3.9796562947729126</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="J6" s="8">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
+        <v>312.61554000000001</v>
+      </c>
+      <c r="L6" s="10">
+        <f>$K$4/K6</f>
+        <v>3.9619249574093471</v>
+      </c>
+      <c r="N6" s="8">
+        <v>4</v>
+      </c>
+      <c r="O6" s="2">
+        <v>959.87148999999999</v>
+      </c>
+      <c r="P6" s="10">
+        <f>$O$4/O6</f>
+        <v>3.9641454711817725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>804.27999</v>
+      </c>
+      <c r="C7" s="10">
+        <f>$B$4/B7</f>
+        <v>7.8881781330901939</v>
+      </c>
+      <c r="D7" s="2">
+        <v>763.15341000000001</v>
+      </c>
+      <c r="E7" s="10">
+        <f>$D$4/D7</f>
+        <v>8.0051714897008726</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="J7" s="8">
+        <v>8</v>
+      </c>
+      <c r="K7" s="2">
+        <v>157.44566</v>
+      </c>
+      <c r="L7" s="10">
+        <f>$K$4/K7</f>
+        <v>7.8665827308291636</v>
+      </c>
+      <c r="N7" s="8">
+        <v>8</v>
+      </c>
+      <c r="O7" s="2">
+        <v>481.52929</v>
+      </c>
+      <c r="P7" s="10">
+        <f>$O$4/O7</f>
+        <v>7.9020535178659639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>416.85750000000002</v>
+      </c>
+      <c r="C8" s="10">
+        <f>$B$4/B8</f>
+        <v>15.219358725703627</v>
+      </c>
+      <c r="D8" s="2">
+        <v>400.87011000000001</v>
+      </c>
+      <c r="E8" s="10">
+        <f>$D$4/D8</f>
+        <v>15.239784078688231</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="J8" s="8">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2">
+        <v>82.123540000000006</v>
+      </c>
+      <c r="L8" s="10">
+        <f>$K$4/K8</f>
+        <v>15.081660020987892</v>
+      </c>
+      <c r="N8" s="8">
+        <v>16</v>
+      </c>
+      <c r="O8" s="2">
+        <v>252.37853000000001</v>
+      </c>
+      <c r="P8" s="10">
+        <f>$O$4/O8</f>
+        <v>15.076838033726562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27">
+        <v>32</v>
+      </c>
+      <c r="B9" s="12">
+        <v>227.58150000000001</v>
+      </c>
+      <c r="C9" s="13">
+        <f>$B$4/B9</f>
+        <v>27.877063074107514</v>
+      </c>
+      <c r="D9" s="12">
+        <v>214.18790000000001</v>
+      </c>
+      <c r="E9" s="13">
+        <f>$D$4/D9</f>
+        <v>28.522497862857797</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="J9" s="11">
+        <v>32</v>
+      </c>
+      <c r="K9" s="12">
+        <v>45.179659999999998</v>
+      </c>
+      <c r="L9" s="13">
+        <f>$K$4/K9</f>
+        <v>27.414090986961835</v>
+      </c>
+      <c r="N9" s="11">
+        <v>32</v>
+      </c>
+      <c r="O9" s="12">
+        <v>135.40665999999999</v>
+      </c>
+      <c r="P9" s="13">
+        <f>$O$4/O9</f>
+        <v>28.101056624541219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="21"/>
+      <c r="P12" s="22"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="16"/>
+      <c r="N13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>225.50916000000001</v>
+      </c>
+      <c r="D14" s="9">
+        <f>$C$14/C14</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1552.02189</v>
+      </c>
+      <c r="H14" s="10">
+        <f>$G$14/G14</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="8">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>4992.0573599999998</v>
+      </c>
+      <c r="L14" s="10">
+        <f>$K$14/K14</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1528.09917</v>
+      </c>
+      <c r="P14" s="10">
+        <f>$O$14/O14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>113.95151</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" ref="D15:D19" si="0">$C$14/C15</f>
+        <v>1.9789922924233301</v>
+      </c>
+      <c r="F15" s="8">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>782.59691999999995</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" ref="H15:H19" si="1">$G$14/G15</f>
+        <v>1.9831689217483761</v>
+      </c>
+      <c r="J15" s="8">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2489.4723800000002</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" ref="L15:L19" si="2">$K$14/K15</f>
+        <v>2.0052672205184296</v>
+      </c>
+      <c r="N15" s="8">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>760.24554000000001</v>
+      </c>
+      <c r="P15" s="10">
+        <f t="shared" ref="P15:P19" si="3">$O$14/O15</f>
+        <v>2.0100074115528517</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>57.761960000000002</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
+        <v>3.9041119795796404</v>
+      </c>
+      <c r="F16" s="8">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2">
+        <v>391.79863999999998</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="1"/>
+        <v>3.9612743168276441</v>
+      </c>
+      <c r="J16" s="8">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1251.8728799999999</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="2"/>
+        <v>3.9876711443737003</v>
+      </c>
+      <c r="N16" s="8">
+        <v>4</v>
+      </c>
+      <c r="O16" s="2">
+        <v>384.14166</v>
+      </c>
+      <c r="P16" s="10">
+        <f t="shared" si="3"/>
+        <v>3.977957428517386</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2">
+        <v>29.097989999999999</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>7.7499909787583272</v>
+      </c>
+      <c r="F17" s="8">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2">
+        <v>198.25934000000001</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="1"/>
+        <v>7.8282409797187862</v>
+      </c>
+      <c r="J17" s="8">
+        <v>8</v>
+      </c>
+      <c r="K17" s="2">
+        <v>637.38895000000002</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="2"/>
+        <v>7.8320425228582948</v>
+      </c>
+      <c r="N17" s="8">
+        <v>8</v>
+      </c>
+      <c r="O17" s="2">
+        <v>193.59109000000001</v>
+      </c>
+      <c r="P17" s="10">
+        <f t="shared" si="3"/>
+        <v>7.8934375027280437</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
+        <v>15.266859999999999</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
+        <v>14.771155299780048</v>
+      </c>
+      <c r="F18" s="8">
+        <v>16</v>
+      </c>
+      <c r="G18" s="2">
+        <v>104.86624</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="1"/>
+        <v>14.80001466630252</v>
+      </c>
+      <c r="J18" s="8">
+        <v>16</v>
+      </c>
+      <c r="K18" s="2">
+        <v>330.64924000000002</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="2"/>
+        <v>15.097743336715364</v>
+      </c>
+      <c r="N18" s="8">
+        <v>16</v>
+      </c>
+      <c r="O18" s="2">
+        <v>102.10281000000001</v>
+      </c>
+      <c r="P18" s="10">
+        <f t="shared" si="3"/>
+        <v>14.966279282617196</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="11">
+        <v>32</v>
+      </c>
+      <c r="C19" s="12">
+        <v>9.0215899999999998</v>
+      </c>
+      <c r="D19" s="19">
+        <f t="shared" si="0"/>
+        <v>24.996609245155234</v>
+      </c>
+      <c r="F19" s="11">
+        <v>32</v>
+      </c>
+      <c r="G19" s="12">
+        <v>56.578319999999998</v>
+      </c>
+      <c r="H19" s="13">
+        <f t="shared" si="1"/>
+        <v>27.431388736887204</v>
+      </c>
+      <c r="J19" s="11">
+        <v>32</v>
+      </c>
+      <c r="K19" s="12">
+        <v>181.62129999999999</v>
+      </c>
+      <c r="L19" s="13">
+        <f t="shared" si="2"/>
+        <v>27.486078780407365</v>
+      </c>
+      <c r="N19" s="11">
+        <v>32</v>
+      </c>
+      <c r="O19" s="12">
+        <v>54.212049999999998</v>
+      </c>
+      <c r="P19" s="13">
+        <f t="shared" si="3"/>
+        <v>28.187444857739195</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="21"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+    </row>
+    <row r="23" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="16"/>
+      <c r="J23" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M23" s="16"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1091.72983</v>
+      </c>
+      <c r="D24" s="10">
+        <f>$C$24/C24</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>6185.4213300000001</v>
+      </c>
+      <c r="H24" s="10">
+        <f>$G$24/G24</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="8">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>5918.1324000000004</v>
+      </c>
+      <c r="L24" s="10">
+        <f>$K$24/K24</f>
+        <v>1</v>
+      </c>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>549.53049999999996</v>
+      </c>
+      <c r="D25" s="10">
+        <f t="shared" ref="D25:D29" si="4">$C$24/C25</f>
+        <v>1.9866592118180886</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3143.5584100000001</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" ref="H25:H29" si="5">$G$24/G25</f>
+        <v>1.9676495624587425</v>
+      </c>
+      <c r="J25" s="8">
+        <v>2</v>
+      </c>
+      <c r="K25" s="2">
+        <v>2992.4668000000001</v>
+      </c>
+      <c r="L25" s="10">
+        <f t="shared" ref="L25:L29" si="6">$K$24/K25</f>
+        <v>1.9776768784870062</v>
+      </c>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2">
+        <v>278.34055000000001</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" si="4"/>
+        <v>3.9222809252909787</v>
+      </c>
+      <c r="F26" s="8">
+        <v>4</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1558.1304399999999</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="5"/>
+        <v>3.9697711893748768</v>
+      </c>
+      <c r="J26" s="8">
+        <v>4</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1484.01116</v>
+      </c>
+      <c r="L26" s="10">
+        <f t="shared" si="6"/>
+        <v>3.9879298481825436</v>
+      </c>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2">
+        <v>140.59107</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="4"/>
+        <v>7.765285732586003</v>
+      </c>
+      <c r="F27" s="8">
+        <v>8</v>
+      </c>
+      <c r="G27" s="2">
+        <v>790.47394999999995</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="5"/>
+        <v>7.8249527767486846</v>
+      </c>
+      <c r="J27" s="8">
+        <v>8</v>
+      </c>
+      <c r="K27" s="2">
+        <v>754.23893999999996</v>
+      </c>
+      <c r="L27" s="10">
+        <f t="shared" si="6"/>
+        <v>7.8464954355180874</v>
+      </c>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>16</v>
+      </c>
+      <c r="C28" s="2">
+        <v>72.71696</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="4"/>
+        <v>15.013414064614363</v>
+      </c>
+      <c r="F28" s="8">
+        <v>16</v>
+      </c>
+      <c r="G28" s="2">
+        <v>406.64362</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="5"/>
+        <v>15.210914485760284</v>
+      </c>
+      <c r="J28" s="8">
+        <v>16</v>
+      </c>
+      <c r="K28" s="2">
+        <v>390.88560000000001</v>
+      </c>
+      <c r="L28" s="10">
+        <f t="shared" si="6"/>
+        <v>15.140318292615538</v>
+      </c>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+    </row>
+    <row r="29" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="11">
+        <v>32</v>
+      </c>
+      <c r="C29" s="12">
+        <v>40.928080000000001</v>
+      </c>
+      <c r="D29" s="13">
+        <f t="shared" si="4"/>
+        <v>26.674347538413723</v>
+      </c>
+      <c r="F29" s="11">
+        <v>32</v>
+      </c>
+      <c r="G29" s="12">
+        <v>218.93725000000001</v>
+      </c>
+      <c r="H29" s="13">
+        <f t="shared" si="5"/>
+        <v>28.252028058267836</v>
+      </c>
+      <c r="J29" s="11">
+        <v>32</v>
+      </c>
+      <c r="K29" s="12">
+        <v>210.65416999999999</v>
+      </c>
+      <c r="L29" s="13">
+        <f t="shared" si="6"/>
+        <v>28.094067162306832</v>
+      </c>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="N12:P12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593AA23E-9CFC-41E5-A923-4F16F489D36A}">
+  <dimension ref="A1:AB25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="25" width="8.7109375" customWidth="1"/>
+    <col min="26" max="26" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="97"/>
+      <c r="E2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="49"/>
+      <c r="I2" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="55"/>
+      <c r="K2" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="91"/>
+      <c r="M2" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="67"/>
+      <c r="O2" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="79"/>
+      <c r="S2" s="84" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="85"/>
+      <c r="U2" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="61"/>
+      <c r="W2" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="91"/>
+      <c r="Z2" s="140" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="143"/>
+      <c r="B3" s="138" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="144" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="118" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="119" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="120" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="122" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="124" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="125" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="126" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="129" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="130" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="131" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="134" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" s="125" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="126" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="141"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B4" s="137">
+        <v>1</v>
+      </c>
+      <c r="C4" s="98">
+        <v>6344.3038299999998</v>
+      </c>
+      <c r="D4" s="99">
+        <f>$C$4/C4</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="100">
+        <v>6109.1739200000002</v>
+      </c>
+      <c r="F4" s="101">
+        <f>$E$4/E4</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="102">
+        <v>1238.5593100000001</v>
+      </c>
+      <c r="H4" s="103">
+        <f>$G$4/G4</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="104">
+        <v>3805.0702200000001</v>
+      </c>
+      <c r="J4" s="105">
+        <f>$I$4/I4</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="106">
+        <v>225.50916000000001</v>
+      </c>
+      <c r="L4" s="107">
+        <f>$K$4/K4</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="108">
+        <v>1552.02189</v>
+      </c>
+      <c r="N4" s="109">
+        <f>$M$4/M4</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="110">
+        <v>4992.0573599999998</v>
+      </c>
+      <c r="P4" s="111">
+        <f>$O$4/O4</f>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="112">
+        <v>1528.09917</v>
+      </c>
+      <c r="R4" s="113">
+        <f>$Q$4/Q4</f>
+        <v>1</v>
+      </c>
+      <c r="S4" s="114">
+        <v>1091.72983</v>
+      </c>
+      <c r="T4" s="115">
+        <f>$S$4/S4</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="116">
+        <v>6185.4213300000001</v>
+      </c>
+      <c r="V4" s="117">
+        <f>$U$4/U4</f>
+        <v>1</v>
+      </c>
+      <c r="W4" s="106">
+        <v>5918.1324000000004</v>
+      </c>
+      <c r="X4" s="107">
+        <f>$W$4/W4</f>
+        <v>1</v>
+      </c>
+      <c r="Z4" s="142">
+        <f>AVERAGE(D4,F4,H4,J4,L4,N4,P4,R4,T4,V4,X4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B5" s="36">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38">
+        <v>3211.6042600000001</v>
+      </c>
+      <c r="D5" s="39">
+        <f t="shared" ref="D5:D9" si="0">$C$4/C5</f>
+        <v>1.9754313783355113</v>
+      </c>
+      <c r="E5" s="44">
+        <v>3009.9733200000001</v>
+      </c>
+      <c r="F5" s="45">
+        <f t="shared" ref="F5:F9" si="1">$E$4/E5</f>
+        <v>2.0296438773749661</v>
+      </c>
+      <c r="G5" s="50">
+        <v>635.85972000000004</v>
+      </c>
+      <c r="H5" s="51">
+        <f t="shared" ref="H5:H9" si="2">$G$4/G5</f>
+        <v>1.9478499282829238</v>
+      </c>
+      <c r="I5" s="56">
+        <v>1904.85754</v>
+      </c>
+      <c r="J5" s="57">
+        <f t="shared" ref="J5:J9" si="3">$I$4/I5</f>
+        <v>1.997561570929866</v>
+      </c>
+      <c r="K5" s="92">
+        <v>113.95151</v>
+      </c>
+      <c r="L5" s="93">
+        <f t="shared" ref="L5:L9" si="4">$K$4/K5</f>
+        <v>1.9789922924233301</v>
+      </c>
+      <c r="M5" s="68">
+        <v>782.59691999999995</v>
+      </c>
+      <c r="N5" s="69">
+        <f t="shared" ref="N5:N9" si="5">$M$4/M5</f>
+        <v>1.9831689217483761</v>
+      </c>
+      <c r="O5" s="74">
+        <v>2489.4723800000002</v>
+      </c>
+      <c r="P5" s="75">
+        <f t="shared" ref="P5:P9" si="6">$O$4/O5</f>
+        <v>2.0052672205184296</v>
+      </c>
+      <c r="Q5" s="80">
+        <v>760.24554000000001</v>
+      </c>
+      <c r="R5" s="81">
+        <f t="shared" ref="R5:R9" si="7">$Q$4/Q5</f>
+        <v>2.0100074115528517</v>
+      </c>
+      <c r="S5" s="86">
+        <v>549.53049999999996</v>
+      </c>
+      <c r="T5" s="87">
+        <f t="shared" ref="T5:T9" si="8">$S$4/S5</f>
+        <v>1.9866592118180886</v>
+      </c>
+      <c r="U5" s="62">
+        <v>3143.5584100000001</v>
+      </c>
+      <c r="V5" s="63">
+        <f t="shared" ref="V5:V9" si="9">$U$4/U5</f>
+        <v>1.9676495624587425</v>
+      </c>
+      <c r="W5" s="92">
+        <v>2992.4668000000001</v>
+      </c>
+      <c r="X5" s="93">
+        <f t="shared" ref="X5:X9" si="10">$W$4/W5</f>
+        <v>1.9776768784870062</v>
+      </c>
+      <c r="Z5" s="142">
+        <f t="shared" ref="Z5:Z9" si="11">AVERAGE(D5,F5,H5,J5,L5,N5,P5,R5,T5,V5,X5)</f>
+        <v>1.9872643867209177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B6" s="36">
+        <v>4</v>
+      </c>
+      <c r="C6" s="38">
+        <v>1581.87771</v>
+      </c>
+      <c r="D6" s="39">
+        <f t="shared" si="0"/>
+        <v>4.0106158585419349</v>
+      </c>
+      <c r="E6" s="44">
+        <v>1535.1008899999999</v>
+      </c>
+      <c r="F6" s="45">
+        <f t="shared" si="1"/>
+        <v>3.9796562947729126</v>
+      </c>
+      <c r="G6" s="50">
+        <v>312.61554000000001</v>
+      </c>
+      <c r="H6" s="51">
+        <f t="shared" si="2"/>
+        <v>3.9619249574093471</v>
+      </c>
+      <c r="I6" s="56">
+        <v>959.87148999999999</v>
+      </c>
+      <c r="J6" s="57">
+        <f t="shared" si="3"/>
+        <v>3.9641454711817725</v>
+      </c>
+      <c r="K6" s="92">
+        <v>57.761960000000002</v>
+      </c>
+      <c r="L6" s="93">
+        <f t="shared" si="4"/>
+        <v>3.9041119795796404</v>
+      </c>
+      <c r="M6" s="68">
+        <v>391.79863999999998</v>
+      </c>
+      <c r="N6" s="69">
+        <f t="shared" si="5"/>
+        <v>3.9612743168276441</v>
+      </c>
+      <c r="O6" s="74">
+        <v>1251.8728799999999</v>
+      </c>
+      <c r="P6" s="75">
+        <f t="shared" si="6"/>
+        <v>3.9876711443737003</v>
+      </c>
+      <c r="Q6" s="80">
+        <v>384.14166</v>
+      </c>
+      <c r="R6" s="81">
+        <f t="shared" si="7"/>
+        <v>3.977957428517386</v>
+      </c>
+      <c r="S6" s="86">
+        <v>278.34055000000001</v>
+      </c>
+      <c r="T6" s="87">
+        <f t="shared" si="8"/>
+        <v>3.9222809252909787</v>
+      </c>
+      <c r="U6" s="62">
+        <v>1558.1304399999999</v>
+      </c>
+      <c r="V6" s="63">
+        <f t="shared" si="9"/>
+        <v>3.9697711893748768</v>
+      </c>
+      <c r="W6" s="92">
+        <v>1484.01116</v>
+      </c>
+      <c r="X6" s="93">
+        <f t="shared" si="10"/>
+        <v>3.9879298481825436</v>
+      </c>
+      <c r="Z6" s="142">
+        <f t="shared" si="11"/>
+        <v>3.9661217649138849</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B7" s="36">
+        <v>8</v>
+      </c>
+      <c r="C7" s="38">
+        <v>804.27999</v>
+      </c>
+      <c r="D7" s="39">
+        <f t="shared" si="0"/>
+        <v>7.8881781330901939</v>
+      </c>
+      <c r="E7" s="44">
+        <v>763.15341000000001</v>
+      </c>
+      <c r="F7" s="45">
+        <f t="shared" si="1"/>
+        <v>8.0051714897008726</v>
+      </c>
+      <c r="G7" s="50">
+        <v>157.44566</v>
+      </c>
+      <c r="H7" s="51">
+        <f t="shared" si="2"/>
+        <v>7.8665827308291636</v>
+      </c>
+      <c r="I7" s="56">
+        <v>481.52929</v>
+      </c>
+      <c r="J7" s="57">
+        <f t="shared" si="3"/>
+        <v>7.9020535178659639</v>
+      </c>
+      <c r="K7" s="92">
+        <v>29.097989999999999</v>
+      </c>
+      <c r="L7" s="93">
+        <f t="shared" si="4"/>
+        <v>7.7499909787583272</v>
+      </c>
+      <c r="M7" s="68">
+        <v>198.25934000000001</v>
+      </c>
+      <c r="N7" s="69">
+        <f t="shared" si="5"/>
+        <v>7.8282409797187862</v>
+      </c>
+      <c r="O7" s="74">
+        <v>637.38895000000002</v>
+      </c>
+      <c r="P7" s="75">
+        <f t="shared" si="6"/>
+        <v>7.8320425228582948</v>
+      </c>
+      <c r="Q7" s="80">
+        <v>193.59109000000001</v>
+      </c>
+      <c r="R7" s="81">
+        <f t="shared" si="7"/>
+        <v>7.8934375027280437</v>
+      </c>
+      <c r="S7" s="86">
+        <v>140.59107</v>
+      </c>
+      <c r="T7" s="87">
+        <f t="shared" si="8"/>
+        <v>7.765285732586003</v>
+      </c>
+      <c r="U7" s="62">
+        <v>790.47394999999995</v>
+      </c>
+      <c r="V7" s="63">
+        <f t="shared" si="9"/>
+        <v>7.8249527767486846</v>
+      </c>
+      <c r="W7" s="92">
+        <v>754.23893999999996</v>
+      </c>
+      <c r="X7" s="93">
+        <f t="shared" si="10"/>
+        <v>7.8464954355180874</v>
+      </c>
+      <c r="Z7" s="142">
+        <f t="shared" si="11"/>
+        <v>7.8547665273093115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B8" s="36">
+        <v>16</v>
+      </c>
+      <c r="C8" s="38">
+        <v>416.85750000000002</v>
+      </c>
+      <c r="D8" s="39">
+        <f t="shared" si="0"/>
+        <v>15.219358725703627</v>
+      </c>
+      <c r="E8" s="44">
+        <v>400.87011000000001</v>
+      </c>
+      <c r="F8" s="45">
+        <f t="shared" si="1"/>
+        <v>15.239784078688231</v>
+      </c>
+      <c r="G8" s="50">
+        <v>82.123540000000006</v>
+      </c>
+      <c r="H8" s="51">
+        <f t="shared" si="2"/>
+        <v>15.081660020987892</v>
+      </c>
+      <c r="I8" s="56">
+        <v>252.37853000000001</v>
+      </c>
+      <c r="J8" s="57">
+        <f t="shared" si="3"/>
+        <v>15.076838033726562</v>
+      </c>
+      <c r="K8" s="92">
+        <v>15.266859999999999</v>
+      </c>
+      <c r="L8" s="93">
+        <f t="shared" si="4"/>
+        <v>14.771155299780048</v>
+      </c>
+      <c r="M8" s="68">
+        <v>104.86624</v>
+      </c>
+      <c r="N8" s="69">
+        <f t="shared" si="5"/>
+        <v>14.80001466630252</v>
+      </c>
+      <c r="O8" s="74">
+        <v>330.64924000000002</v>
+      </c>
+      <c r="P8" s="75">
+        <f t="shared" si="6"/>
+        <v>15.097743336715364</v>
+      </c>
+      <c r="Q8" s="80">
+        <v>102.10281000000001</v>
+      </c>
+      <c r="R8" s="81">
+        <f t="shared" si="7"/>
+        <v>14.966279282617196</v>
+      </c>
+      <c r="S8" s="86">
+        <v>72.71696</v>
+      </c>
+      <c r="T8" s="87">
+        <f t="shared" si="8"/>
+        <v>15.013414064614363</v>
+      </c>
+      <c r="U8" s="62">
+        <v>406.64362</v>
+      </c>
+      <c r="V8" s="63">
+        <f t="shared" si="9"/>
+        <v>15.210914485760284</v>
+      </c>
+      <c r="W8" s="92">
+        <v>390.88560000000001</v>
+      </c>
+      <c r="X8" s="93">
+        <f t="shared" si="10"/>
+        <v>15.140318292615538</v>
+      </c>
+      <c r="Z8" s="142">
+        <f t="shared" si="11"/>
+        <v>15.056134571591963</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="37">
+        <v>32</v>
+      </c>
+      <c r="C9" s="40">
+        <v>227.58150000000001</v>
+      </c>
+      <c r="D9" s="41">
+        <f t="shared" si="0"/>
+        <v>27.877063074107514</v>
+      </c>
+      <c r="E9" s="46">
+        <v>214.18790000000001</v>
+      </c>
+      <c r="F9" s="47">
+        <f t="shared" si="1"/>
+        <v>28.522497862857797</v>
+      </c>
+      <c r="G9" s="52">
+        <v>45.179659999999998</v>
+      </c>
+      <c r="H9" s="53">
+        <f t="shared" si="2"/>
+        <v>27.414090986961835</v>
+      </c>
+      <c r="I9" s="58">
+        <v>135.40665999999999</v>
+      </c>
+      <c r="J9" s="59">
+        <f t="shared" si="3"/>
+        <v>28.101056624541219</v>
+      </c>
+      <c r="K9" s="94">
+        <v>9.0215899999999998</v>
+      </c>
+      <c r="L9" s="95">
+        <f t="shared" si="4"/>
+        <v>24.996609245155234</v>
+      </c>
+      <c r="M9" s="70">
+        <v>56.578319999999998</v>
+      </c>
+      <c r="N9" s="71">
+        <f t="shared" si="5"/>
+        <v>27.431388736887204</v>
+      </c>
+      <c r="O9" s="76">
+        <v>181.62129999999999</v>
+      </c>
+      <c r="P9" s="77">
+        <f t="shared" si="6"/>
+        <v>27.486078780407365</v>
+      </c>
+      <c r="Q9" s="82">
+        <v>54.212049999999998</v>
+      </c>
+      <c r="R9" s="83">
+        <f t="shared" si="7"/>
+        <v>28.187444857739195</v>
+      </c>
+      <c r="S9" s="88">
+        <v>40.928080000000001</v>
+      </c>
+      <c r="T9" s="89">
+        <f t="shared" si="8"/>
+        <v>26.674347538413723</v>
+      </c>
+      <c r="U9" s="64">
+        <v>218.93725000000001</v>
+      </c>
+      <c r="V9" s="65">
+        <f t="shared" si="9"/>
+        <v>28.252028058267836</v>
+      </c>
+      <c r="W9" s="94">
+        <v>210.65416999999999</v>
+      </c>
+      <c r="X9" s="95">
+        <f t="shared" si="10"/>
+        <v>28.094067162306832</v>
+      </c>
+      <c r="Z9" s="142">
+        <f t="shared" si="11"/>
+        <v>27.548788447967794</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="148"/>
+      <c r="C12" s="149" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="149" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="149" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="149" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="149" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="149" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="149" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="149" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="149" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="149" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="150" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="139"/>
+      <c r="P12" s="156" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="146">
+        <v>0</v>
+      </c>
+      <c r="D13" s="145">
+        <v>3.708501</v>
+      </c>
+      <c r="E13" s="145">
+        <v>11.017976000000001</v>
+      </c>
+      <c r="F13" s="145">
+        <v>15.069315</v>
+      </c>
+      <c r="G13" s="145">
+        <v>8.8101599999999998</v>
+      </c>
+      <c r="H13" s="145">
+        <v>15.717249000000001</v>
+      </c>
+      <c r="I13" s="145">
+        <v>7.9499180000000003</v>
+      </c>
+      <c r="J13" s="147">
+        <v>3.113645</v>
+      </c>
+      <c r="K13" s="145">
+        <v>9.0983169999999998</v>
+      </c>
+      <c r="L13" s="145">
+        <v>12.853278</v>
+      </c>
+      <c r="M13" s="151">
+        <v>15.432489</v>
+      </c>
+      <c r="O13" s="157" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="158">
+        <v>9478</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="147">
+        <v>3.708501</v>
+      </c>
+      <c r="D14" s="146">
+        <v>0</v>
+      </c>
+      <c r="E14" s="145">
+        <v>14.143967999999999</v>
+      </c>
+      <c r="F14" s="145">
+        <v>11.963168</v>
+      </c>
+      <c r="G14" s="145">
+        <v>7.348312</v>
+      </c>
+      <c r="H14" s="145">
+        <v>18.627376999999999</v>
+      </c>
+      <c r="I14" s="145">
+        <v>10.534774000000001</v>
+      </c>
+      <c r="J14" s="145">
+        <v>6.1968019999999999</v>
+      </c>
+      <c r="K14" s="145">
+        <v>9.5868249999999993</v>
+      </c>
+      <c r="L14" s="145">
+        <v>13.231009999999999</v>
+      </c>
+      <c r="M14" s="151">
+        <v>18.51323</v>
+      </c>
+      <c r="O14" s="157" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="158">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="145">
+        <v>11.017976000000001</v>
+      </c>
+      <c r="D15" s="145">
+        <v>14.143967999999999</v>
+      </c>
+      <c r="E15" s="146">
+        <v>0</v>
+      </c>
+      <c r="F15" s="145">
+        <v>26.085691000000001</v>
+      </c>
+      <c r="G15" s="145">
+        <v>16.468078999999999</v>
+      </c>
+      <c r="H15" s="145">
+        <v>6.7052069999999997</v>
+      </c>
+      <c r="I15" s="145">
+        <v>7.9040299999999997</v>
+      </c>
+      <c r="J15" s="145">
+        <v>8.064584</v>
+      </c>
+      <c r="K15" s="145">
+        <v>13.836762999999999</v>
+      </c>
+      <c r="L15" s="145">
+        <v>16.402566</v>
+      </c>
+      <c r="M15" s="152">
+        <v>4.4361519999999999</v>
+      </c>
+      <c r="O15" s="157" t="s">
+        <v>6</v>
+      </c>
+      <c r="P15" s="158">
+        <v>5538</v>
+      </c>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+    </row>
+    <row r="16" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="145">
+        <v>15.069315</v>
+      </c>
+      <c r="D16" s="147">
+        <v>11.963168</v>
+      </c>
+      <c r="E16" s="145">
+        <v>26.085691000000001</v>
+      </c>
+      <c r="F16" s="146">
+        <v>0</v>
+      </c>
+      <c r="G16" s="145">
+        <v>13.412691000000001</v>
+      </c>
+      <c r="H16" s="145">
+        <v>30.326366</v>
+      </c>
+      <c r="I16" s="145">
+        <v>21.746663999999999</v>
+      </c>
+      <c r="J16" s="145">
+        <v>18.150805999999999</v>
+      </c>
+      <c r="K16" s="145">
+        <v>18.257642000000001</v>
+      </c>
+      <c r="L16" s="145">
+        <v>20.360185000000001</v>
+      </c>
+      <c r="M16" s="151">
+        <v>30.473040999999998</v>
+      </c>
+      <c r="O16" s="157" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" s="158">
+        <v>301</v>
+      </c>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+    </row>
+    <row r="17" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="145">
+        <v>8.8101599999999998</v>
+      </c>
+      <c r="D17" s="147">
+        <v>7.348312</v>
+      </c>
+      <c r="E17" s="145">
+        <v>16.468078999999999</v>
+      </c>
+      <c r="F17" s="145">
+        <v>13.412691000000001</v>
+      </c>
+      <c r="G17" s="146">
+        <v>0</v>
+      </c>
+      <c r="H17" s="145">
+        <v>19.365057</v>
+      </c>
+      <c r="I17" s="145">
+        <v>15.565144</v>
+      </c>
+      <c r="J17" s="145">
+        <v>10.072918</v>
+      </c>
+      <c r="K17" s="145">
+        <v>15.235410999999999</v>
+      </c>
+      <c r="L17" s="145">
+        <v>18.560316</v>
+      </c>
+      <c r="M17" s="151">
+        <v>19.901475000000001</v>
+      </c>
+      <c r="O17" s="157" t="s">
+        <v>8</v>
+      </c>
+      <c r="P17" s="158">
+        <v>2135</v>
+      </c>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+    </row>
+    <row r="18" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="145">
+        <v>15.717249000000001</v>
+      </c>
+      <c r="D18" s="145">
+        <v>18.627376999999999</v>
+      </c>
+      <c r="E18" s="145">
+        <v>6.7052069999999997</v>
+      </c>
+      <c r="F18" s="145">
+        <v>30.326366</v>
+      </c>
+      <c r="G18" s="145">
+        <v>19.365057</v>
+      </c>
+      <c r="H18" s="146">
+        <v>0</v>
+      </c>
+      <c r="I18" s="145">
+        <v>14.009862999999999</v>
+      </c>
+      <c r="J18" s="145">
+        <v>12.783825999999999</v>
+      </c>
+      <c r="K18" s="145">
+        <v>19.916284000000001</v>
+      </c>
+      <c r="L18" s="145">
+        <v>22.812947999999999</v>
+      </c>
+      <c r="M18" s="152">
+        <v>5.7946759999999999</v>
+      </c>
+      <c r="O18" s="157" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="158">
+        <v>7573</v>
+      </c>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+    </row>
+    <row r="19" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="145">
+        <v>7.9499180000000003</v>
+      </c>
+      <c r="D19" s="145">
+        <v>10.534774000000001</v>
+      </c>
+      <c r="E19" s="145">
+        <v>7.9040299999999997</v>
+      </c>
+      <c r="F19" s="145">
+        <v>21.746663999999999</v>
+      </c>
+      <c r="G19" s="145">
+        <v>15.565144</v>
+      </c>
+      <c r="H19" s="145">
+        <v>14.009862999999999</v>
+      </c>
+      <c r="I19" s="146">
+        <v>0</v>
+      </c>
+      <c r="J19" s="147">
+        <v>6.5823450000000001</v>
+      </c>
+      <c r="K19" s="145">
+        <v>6.7725020000000002</v>
+      </c>
+      <c r="L19" s="145">
+        <v>8.9502500000000005</v>
+      </c>
+      <c r="M19" s="151">
+        <v>10.982179</v>
+      </c>
+      <c r="O19" s="157" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" s="158">
+        <v>2087</v>
+      </c>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+    </row>
+    <row r="20" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="147">
+        <v>3.113645</v>
+      </c>
+      <c r="D20" s="145">
+        <v>6.1968019999999999</v>
+      </c>
+      <c r="E20" s="145">
+        <v>8.064584</v>
+      </c>
+      <c r="F20" s="145">
+        <v>18.150805999999999</v>
+      </c>
+      <c r="G20" s="145">
+        <v>10.072918</v>
+      </c>
+      <c r="H20" s="145">
+        <v>12.783825999999999</v>
+      </c>
+      <c r="I20" s="145">
+        <v>6.5823450000000001</v>
+      </c>
+      <c r="J20" s="146">
+        <v>0</v>
+      </c>
+      <c r="K20" s="145">
+        <v>9.5082850000000008</v>
+      </c>
+      <c r="L20" s="145">
+        <v>13.17277</v>
+      </c>
+      <c r="M20" s="151">
+        <v>12.330344</v>
+      </c>
+      <c r="O20" s="157" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20" s="158">
+        <v>1480</v>
+      </c>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+    </row>
+    <row r="21" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="145">
+        <v>9.0983169999999998</v>
+      </c>
+      <c r="D21" s="145">
+        <v>9.5868249999999993</v>
+      </c>
+      <c r="E21" s="145">
+        <v>13.836762999999999</v>
+      </c>
+      <c r="F21" s="145">
+        <v>18.257642000000001</v>
+      </c>
+      <c r="G21" s="145">
+        <v>15.235410999999999</v>
+      </c>
+      <c r="H21" s="145">
+        <v>19.916284000000001</v>
+      </c>
+      <c r="I21" s="145">
+        <v>6.7725020000000002</v>
+      </c>
+      <c r="J21" s="145">
+        <v>9.5082850000000008</v>
+      </c>
+      <c r="K21" s="146">
+        <v>0</v>
+      </c>
+      <c r="L21" s="147">
+        <v>3.893904</v>
+      </c>
+      <c r="M21" s="151">
+        <v>16.919685999999999</v>
+      </c>
+      <c r="O21" s="157" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21" s="158">
+        <v>9757</v>
+      </c>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+    </row>
+    <row r="22" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="145">
+        <v>12.853278</v>
+      </c>
+      <c r="D22" s="145">
+        <v>13.231009999999999</v>
+      </c>
+      <c r="E22" s="145">
+        <v>16.402566</v>
+      </c>
+      <c r="F22" s="145">
+        <v>20.360185000000001</v>
+      </c>
+      <c r="G22" s="145">
+        <v>18.560316</v>
+      </c>
+      <c r="H22" s="145">
+        <v>22.812947999999999</v>
+      </c>
+      <c r="I22" s="145">
+        <v>8.9502500000000005</v>
+      </c>
+      <c r="J22" s="145">
+        <v>13.17277</v>
+      </c>
+      <c r="K22" s="147">
+        <v>3.893904</v>
+      </c>
+      <c r="L22" s="146">
+        <v>0</v>
+      </c>
+      <c r="M22" s="151">
+        <v>19.180605</v>
+      </c>
+      <c r="O22" s="157" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="158">
+        <v>9239</v>
+      </c>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+    </row>
+    <row r="23" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="153">
+        <v>15.432489</v>
+      </c>
+      <c r="D23" s="153">
+        <v>18.51323</v>
+      </c>
+      <c r="E23" s="154">
+        <v>4.4361519999999999</v>
+      </c>
+      <c r="F23" s="153">
+        <v>30.473040999999998</v>
+      </c>
+      <c r="G23" s="153">
+        <v>19.901475000000001</v>
+      </c>
+      <c r="H23" s="153">
+        <v>5.7946759999999999</v>
+      </c>
+      <c r="I23" s="153">
+        <v>10.982179</v>
+      </c>
+      <c r="J23" s="153">
+        <v>12.330344</v>
+      </c>
+      <c r="K23" s="153">
+        <v>16.919685999999999</v>
+      </c>
+      <c r="L23" s="153">
+        <v>19.180605</v>
+      </c>
+      <c r="M23" s="155">
+        <v>0</v>
+      </c>
+      <c r="O23" s="157" t="s">
+        <v>4</v>
+      </c>
+      <c r="P23" s="158">
+        <v>10050</v>
+      </c>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W25" s="15"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data changed to sum of all results
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toaxo\Desktop\MSU\Sem5\Hausdorff\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BB5B46-608C-4C26-9521-587451EF996B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D60ECE7-C04B-4673-AC02-AB54F5C4300D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B2AFDC7F-E8CC-4187-9F4B-7A735A4181DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2AFDC7F-E8CC-4187-9F4B-7A735A4181DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="42">
   <si>
     <t>PROCESSES</t>
   </si>
@@ -118,6 +118,51 @@
   </si>
   <si>
     <t>Vertices</t>
+  </si>
+  <si>
+    <t>EFFICIENCY</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>865K</t>
+  </si>
+  <si>
+    <t>135K</t>
+  </si>
+  <si>
+    <t>541K</t>
+  </si>
+  <si>
+    <t>29K</t>
+  </si>
+  <si>
+    <t>209K</t>
+  </si>
+  <si>
+    <t>740K</t>
+  </si>
+  <si>
+    <t>204K</t>
+  </si>
+  <si>
+    <t>145K</t>
+  </si>
+  <si>
+    <t>953K</t>
+  </si>
+  <si>
+    <t>903K</t>
+  </si>
+  <si>
+    <t>982K</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -305,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -708,11 +753,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -737,15 +806,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -757,18 +817,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,102 +836,42 @@
     <xf numFmtId="2" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -965,12 +956,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -997,7 +982,107 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1036,7 +1121,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1046,22 +1131,22 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="tr-TR" b="1">
+              <a:rPr lang="tr-TR" sz="1600" b="1">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>PARALLEL</a:t>
+              <a:t>Parallel </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="tr-TR" b="1" baseline="0">
+              <a:rPr lang="tr-TR" sz="1600" b="1" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> HAUSDORFF DISTANCE</a:t>
+              <a:t>Naive Hausdorff Distance</a:t>
             </a:r>
-            <a:endParaRPr lang="tr-TR" b="1">
+            <a:endParaRPr lang="tr-TR" sz="1600" b="1">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1069,6 +1154,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29476158710283679"/>
+          <c:y val="1.8511073241417677E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1082,7 +1175,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1097,7 +1190,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11702081122852408"/>
+          <c:y val="0.16713312789766924"/>
+          <c:w val="0.80068850855627705"/>
+          <c:h val="0.68833158627994229"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1121,9 +1224,36 @@
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="5000"/>
+                      <a:lumOff val="95000"/>
+                      <a:alpha val="96000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="74000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="45000"/>
+                      <a:lumOff val="55000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="83000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="45000"/>
+                      <a:lumOff val="55000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="30000"/>
+                      <a:lumOff val="70000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1218,22 +1348,22 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6344.3038299999998</c:v>
+                  <c:v>38990.078420000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3211.6042600000001</c:v>
+                  <c:v>19594.116900000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1581.87771</c:v>
+                  <c:v>9795.5229200000012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>804.27999</c:v>
+                  <c:v>4950.0496800000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>416.85750000000002</c:v>
+                  <c:v>2575.3610100000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>227.58150000000001</c:v>
+                  <c:v>1394.3084799999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1276,22 +1406,22 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="diamond"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="C00000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1300,9 +1430,7 @@
           <c:dLbls>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1328,7 +1456,7 @@
                 <a:endParaRPr lang="tr-TR"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1393,19 +1521,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9754313783355113</c:v>
+                  <c:v>1.9898869961319872</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0106158585419349</c:v>
+                  <c:v>3.9803978550641785</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.8881781330901939</c:v>
+                  <c:v>7.8767044657216463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.219358725703627</c:v>
+                  <c:v>15.139655476883998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.877063074107514</c:v>
+                  <c:v>27.963738999851746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,6 +1542,291 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D668-43B0-9241-673A10D19FEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sayfa1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EFFICIENCY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="00B050"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5DC4-4581-B335-2D2E8E4CC121}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.3412592078706002E-3"/>
+                  <c:y val="2.4681430988556789E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-5DC4-4581-B335-2D2E8E4CC121}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1706296039353001E-3"/>
+                  <c:y val="2.46814309885569E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-5DC4-4581-B335-2D2E8E4CC121}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.7766609862126514E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-5DC4-4581-B335-2D2E8E4CC121}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1706296039353001E-3"/>
+                  <c:y val="1.8511073241417677E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-5DC4-4581-B335-2D2E8E4CC121}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5917766545461419E-16"/>
+                  <c:y val="1.5425894367848064E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-5DC4-4581-B335-2D2E8E4CC121}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1706296039351409E-3"/>
+                  <c:y val="1.5425894367848176E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-5DC4-4581-B335-2D2E8E4CC121}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="tr-TR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sayfa1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99494349806599358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99509946376604463</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98458805821520579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9462284673052499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.87386684374536705</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5DC4-4581-B335-2D2E8E4CC121}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1444,7 +1857,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -1454,19 +1867,21 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="tr-TR" sz="1200" b="1">
+                  <a:rPr lang="tr-TR" sz="1400" b="1">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>PROCESSES</a:t>
+                  <a:t>MPI Processes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="bg2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1477,7 +1892,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -1512,7 +1927,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1562,7 +1977,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -1572,20 +1987,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="tr-TR" sz="1200" b="1">
+                  <a:rPr lang="tr-TR" sz="1400" b="1">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>ELAPSED</a:t>
+                  <a:t>Elapsed Time</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="tr-TR" sz="1200" b="1" baseline="0">
+                  <a:rPr lang="tr-TR" sz="1400" b="1" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> TIME (s)</a:t>
+                  <a:t>(s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1594,13 +2009,15 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.2195121951219513E-2"/>
-              <c:y val="0.36859766939546623"/>
+              <c:x val="2.6166764362758519E-3"/>
+              <c:y val="0.38269171179932227"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="bg2"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1611,7 +2028,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -1640,7 +2057,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1669,11 +2086,11 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1686,20 +2103,41 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="tr-TR" sz="1200" b="1">
+                  <a:rPr lang="tr-TR" sz="1400" b="1">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>SPEEDUP</a:t>
+                  <a:t>Speedup</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1400" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> &amp; Efficiency</a:t>
+                </a:r>
+                <a:endParaRPr lang="tr-TR" sz="1400" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.9604137748774324"/>
+              <c:y val="0.35146358676014933"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:sysClr val="window" lastClr="FFFFFF"/>
+              <a:schemeClr val="bg2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1707,11 +2145,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1743,7 +2181,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1790,6 +2228,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2573052592073915"/>
+          <c:y val="8.6662778767133394E-2"/>
+          <c:w val="0.50646197047637176"/>
+          <c:h val="4.1511662927482595E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1805,10 +2253,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2410,16 +2855,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>16564</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352837</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>140806</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>132519</xdr:rowOff>
+      <xdr:colOff>240195</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>149086</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2746,8 +3191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4FF6C2-EC25-4B3E-BCE0-855100FCA57B}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,6 +3200,7 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -2767,16 +3213,23 @@
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>6344.3038299999998</v>
+      <c r="B2" s="74">
+        <v>38990.078420000005</v>
       </c>
       <c r="C2" s="1">
         <f>$B$2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <f>$C2/$A2</f>
         <v>1</v>
       </c>
     </row>
@@ -2784,60 +3237,80 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>3211.6042600000001</v>
+      <c r="B3" s="36">
+        <v>19594.116900000001</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C7" si="0">$B$2/B3</f>
-        <v>1.9754313783355113</v>
+        <v>1.9898869961319872</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D7" si="1">$C3/$A3</f>
+        <v>0.99494349806599358</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>1581.87771</v>
+      <c r="B4" s="36">
+        <v>9795.5229200000012</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="0"/>
-        <v>4.0106158585419349</v>
+        <v>3.9803978550641785</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.99509946376604463</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <v>804.27999</v>
+      <c r="B5" s="36">
+        <v>4950.0496800000001</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="0"/>
-        <v>7.8881781330901939</v>
+        <v>7.8767044657216463</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.98458805821520579</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>16</v>
       </c>
-      <c r="B6" s="2">
-        <v>416.85750000000002</v>
+      <c r="B6" s="36">
+        <v>2575.3610100000001</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>15.219358725703627</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>15.139655476883998</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="1"/>
+        <v>0.9462284673052499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>32</v>
       </c>
-      <c r="B7" s="2">
-        <v>227.58150000000001</v>
+      <c r="B7" s="38">
+        <v>1394.3084799999999</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>27.877063074107514</v>
+        <v>27.963738999851746</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.87386684374536705</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2857,7 +3330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70DCB3C-3F08-4ABF-81AB-DC0E48A72EC9}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J22" sqref="J22:L22"/>
     </sheetView>
   </sheetViews>
@@ -2882,86 +3355,86 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="133"/>
+      <c r="D2" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="135"/>
+      <c r="F2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
       <c r="M2" s="14"/>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="132"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="23"/>
+      <c r="E3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="20"/>
       <c r="I3" s="16"/>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="M3" s="16"/>
-      <c r="N3" s="23" t="s">
+      <c r="N3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="P3" s="22" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="23">
         <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>6344.3038299999998</v>
       </c>
       <c r="C4" s="10">
-        <f>$B$4/B4</f>
+        <f t="shared" ref="C4:C9" si="0">$B$4/B4</f>
         <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>6109.1739200000002</v>
       </c>
       <c r="E4" s="10">
-        <f>$D$4/D4</f>
+        <f t="shared" ref="E4:E9" si="1">$D$4/D4</f>
         <v>1</v>
       </c>
       <c r="F4" s="8"/>
@@ -2972,7 +3445,7 @@
         <v>1238.5593100000001</v>
       </c>
       <c r="L4" s="10">
-        <f>$K$4/K4</f>
+        <f t="shared" ref="L4:L9" si="2">$K$4/K4</f>
         <v>1</v>
       </c>
       <c r="N4" s="8">
@@ -2982,26 +3455,26 @@
         <v>3805.0702200000001</v>
       </c>
       <c r="P4" s="10">
-        <f>$O$4/O4</f>
+        <f t="shared" ref="P4:P9" si="3">$O$4/O4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+      <c r="A5" s="23">
         <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>3211.6042600000001</v>
       </c>
       <c r="C5" s="10">
-        <f>$B$4/B5</f>
+        <f t="shared" si="0"/>
         <v>1.9754313783355113</v>
       </c>
       <c r="D5" s="2">
         <v>3009.9733200000001</v>
       </c>
       <c r="E5" s="10">
-        <f>$D$4/D5</f>
+        <f t="shared" si="1"/>
         <v>2.0296438773749661</v>
       </c>
       <c r="F5" s="8"/>
@@ -3012,7 +3485,7 @@
         <v>635.85972000000004</v>
       </c>
       <c r="L5" s="10">
-        <f>$K$4/K5</f>
+        <f t="shared" si="2"/>
         <v>1.9478499282829238</v>
       </c>
       <c r="N5" s="8">
@@ -3022,26 +3495,26 @@
         <v>1904.85754</v>
       </c>
       <c r="P5" s="10">
-        <f>$O$4/O5</f>
+        <f t="shared" si="3"/>
         <v>1.997561570929866</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="23">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>1581.87771</v>
       </c>
       <c r="C6" s="10">
-        <f>$B$4/B6</f>
+        <f t="shared" si="0"/>
         <v>4.0106158585419349</v>
       </c>
       <c r="D6" s="2">
         <v>1535.1008899999999</v>
       </c>
       <c r="E6" s="10">
-        <f>$D$4/D6</f>
+        <f t="shared" si="1"/>
         <v>3.9796562947729126</v>
       </c>
       <c r="F6" s="8"/>
@@ -3052,7 +3525,7 @@
         <v>312.61554000000001</v>
       </c>
       <c r="L6" s="10">
-        <f>$K$4/K6</f>
+        <f t="shared" si="2"/>
         <v>3.9619249574093471</v>
       </c>
       <c r="N6" s="8">
@@ -3062,26 +3535,26 @@
         <v>959.87148999999999</v>
       </c>
       <c r="P6" s="10">
-        <f>$O$4/O6</f>
+        <f t="shared" si="3"/>
         <v>3.9641454711817725</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+      <c r="A7" s="23">
         <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>804.27999</v>
       </c>
       <c r="C7" s="10">
-        <f>$B$4/B7</f>
+        <f t="shared" si="0"/>
         <v>7.8881781330901939</v>
       </c>
       <c r="D7" s="2">
         <v>763.15341000000001</v>
       </c>
       <c r="E7" s="10">
-        <f>$D$4/D7</f>
+        <f t="shared" si="1"/>
         <v>8.0051714897008726</v>
       </c>
       <c r="F7" s="8"/>
@@ -3092,7 +3565,7 @@
         <v>157.44566</v>
       </c>
       <c r="L7" s="10">
-        <f>$K$4/K7</f>
+        <f t="shared" si="2"/>
         <v>7.8665827308291636</v>
       </c>
       <c r="N7" s="8">
@@ -3102,26 +3575,26 @@
         <v>481.52929</v>
       </c>
       <c r="P7" s="10">
-        <f>$O$4/O7</f>
+        <f t="shared" si="3"/>
         <v>7.9020535178659639</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="23">
         <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>416.85750000000002</v>
       </c>
       <c r="C8" s="10">
-        <f>$B$4/B8</f>
+        <f t="shared" si="0"/>
         <v>15.219358725703627</v>
       </c>
       <c r="D8" s="2">
         <v>400.87011000000001</v>
       </c>
       <c r="E8" s="10">
-        <f>$D$4/D8</f>
+        <f t="shared" si="1"/>
         <v>15.239784078688231</v>
       </c>
       <c r="F8" s="8"/>
@@ -3132,7 +3605,7 @@
         <v>82.123540000000006</v>
       </c>
       <c r="L8" s="10">
-        <f>$K$4/K8</f>
+        <f t="shared" si="2"/>
         <v>15.081660020987892</v>
       </c>
       <c r="N8" s="8">
@@ -3142,26 +3615,26 @@
         <v>252.37853000000001</v>
       </c>
       <c r="P8" s="10">
-        <f>$O$4/O8</f>
+        <f t="shared" si="3"/>
         <v>15.076838033726562</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
+      <c r="A9" s="24">
         <v>32</v>
       </c>
       <c r="B9" s="12">
         <v>227.58150000000001</v>
       </c>
       <c r="C9" s="13">
-        <f>$B$4/B9</f>
+        <f t="shared" si="0"/>
         <v>27.877063074107514</v>
       </c>
       <c r="D9" s="12">
         <v>214.18790000000001</v>
       </c>
       <c r="E9" s="13">
-        <f>$D$4/D9</f>
+        <f t="shared" si="1"/>
         <v>28.522497862857797</v>
       </c>
       <c r="F9" s="11"/>
@@ -3172,7 +3645,7 @@
         <v>45.179659999999998</v>
       </c>
       <c r="L9" s="13">
-        <f>$K$4/K9</f>
+        <f t="shared" si="2"/>
         <v>27.414090986961835</v>
       </c>
       <c r="N9" s="11">
@@ -3182,74 +3655,74 @@
         <v>135.40665999999999</v>
       </c>
       <c r="P9" s="13">
-        <f>$O$4/O9</f>
+        <f t="shared" si="3"/>
         <v>28.101056624541219</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="132"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
+      <c r="G12" s="131"/>
+      <c r="H12" s="132"/>
       <c r="I12" s="14"/>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="21"/>
-      <c r="L12" s="22"/>
+      <c r="K12" s="131"/>
+      <c r="L12" s="132"/>
       <c r="M12" s="14"/>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="O12" s="21"/>
-      <c r="P12" s="22"/>
+      <c r="O12" s="131"/>
+      <c r="P12" s="132"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="16"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="22" t="s">
         <v>1</v>
       </c>
       <c r="I13" s="16"/>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="22" t="s">
         <v>1</v>
       </c>
       <c r="M13" s="16"/>
-      <c r="N13" s="23" t="s">
+      <c r="N13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="24" t="s">
+      <c r="O13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="22" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3303,7 +3776,7 @@
         <v>113.95151</v>
       </c>
       <c r="D15" s="9">
-        <f t="shared" ref="D15:D19" si="0">$C$14/C15</f>
+        <f t="shared" ref="D15:D19" si="4">$C$14/C15</f>
         <v>1.9789922924233301</v>
       </c>
       <c r="F15" s="8">
@@ -3313,7 +3786,7 @@
         <v>782.59691999999995</v>
       </c>
       <c r="H15" s="10">
-        <f t="shared" ref="H15:H19" si="1">$G$14/G15</f>
+        <f t="shared" ref="H15:H19" si="5">$G$14/G15</f>
         <v>1.9831689217483761</v>
       </c>
       <c r="J15" s="8">
@@ -3323,7 +3796,7 @@
         <v>2489.4723800000002</v>
       </c>
       <c r="L15" s="10">
-        <f t="shared" ref="L15:L19" si="2">$K$14/K15</f>
+        <f t="shared" ref="L15:L19" si="6">$K$14/K15</f>
         <v>2.0052672205184296</v>
       </c>
       <c r="N15" s="8">
@@ -3333,7 +3806,7 @@
         <v>760.24554000000001</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" ref="P15:P19" si="3">$O$14/O15</f>
+        <f t="shared" ref="P15:P19" si="7">$O$14/O15</f>
         <v>2.0100074115528517</v>
       </c>
     </row>
@@ -3345,7 +3818,7 @@
         <v>57.761960000000002</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.9041119795796404</v>
       </c>
       <c r="F16" s="8">
@@ -3355,7 +3828,7 @@
         <v>391.79863999999998</v>
       </c>
       <c r="H16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.9612743168276441</v>
       </c>
       <c r="J16" s="8">
@@ -3365,7 +3838,7 @@
         <v>1251.8728799999999</v>
       </c>
       <c r="L16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.9876711443737003</v>
       </c>
       <c r="N16" s="8">
@@ -3375,7 +3848,7 @@
         <v>384.14166</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.977957428517386</v>
       </c>
     </row>
@@ -3387,7 +3860,7 @@
         <v>29.097989999999999</v>
       </c>
       <c r="D17" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7.7499909787583272</v>
       </c>
       <c r="F17" s="8">
@@ -3397,7 +3870,7 @@
         <v>198.25934000000001</v>
       </c>
       <c r="H17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.8282409797187862</v>
       </c>
       <c r="J17" s="8">
@@ -3407,7 +3880,7 @@
         <v>637.38895000000002</v>
       </c>
       <c r="L17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7.8320425228582948</v>
       </c>
       <c r="N17" s="8">
@@ -3417,7 +3890,7 @@
         <v>193.59109000000001</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7.8934375027280437</v>
       </c>
     </row>
@@ -3429,7 +3902,7 @@
         <v>15.266859999999999</v>
       </c>
       <c r="D18" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14.771155299780048</v>
       </c>
       <c r="F18" s="8">
@@ -3439,7 +3912,7 @@
         <v>104.86624</v>
       </c>
       <c r="H18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14.80001466630252</v>
       </c>
       <c r="J18" s="8">
@@ -3449,7 +3922,7 @@
         <v>330.64924000000002</v>
       </c>
       <c r="L18" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>15.097743336715364</v>
       </c>
       <c r="N18" s="8">
@@ -3459,7 +3932,7 @@
         <v>102.10281000000001</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>14.966279282617196</v>
       </c>
     </row>
@@ -3471,7 +3944,7 @@
         <v>9.0215899999999998</v>
       </c>
       <c r="D19" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>24.996609245155234</v>
       </c>
       <c r="F19" s="11">
@@ -3481,7 +3954,7 @@
         <v>56.578319999999998</v>
       </c>
       <c r="H19" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>27.431388736887204</v>
       </c>
       <c r="J19" s="11">
@@ -3491,7 +3964,7 @@
         <v>181.62129999999999</v>
       </c>
       <c r="L19" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>27.486078780407365</v>
       </c>
       <c r="N19" s="11">
@@ -3501,7 +3974,7 @@
         <v>54.212049999999998</v>
       </c>
       <c r="P19" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28.187444857739195</v>
       </c>
     </row>
@@ -3511,56 +3984,56 @@
       <c r="R21" s="18"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
+      <c r="C22" s="131"/>
+      <c r="D22" s="132"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
+      <c r="G22" s="131"/>
+      <c r="H22" s="132"/>
       <c r="I22" s="14"/>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="21"/>
-      <c r="L22" s="22"/>
+      <c r="K22" s="131"/>
+      <c r="L22" s="132"/>
       <c r="M22" s="14"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
     </row>
     <row r="23" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="16"/>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="22" t="s">
         <v>1</v>
       </c>
       <c r="I23" s="16"/>
-      <c r="J23" s="23" t="s">
+      <c r="J23" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K23" s="24" t="s">
+      <c r="K23" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="L23" s="25" t="s">
+      <c r="L23" s="22" t="s">
         <v>1</v>
       </c>
       <c r="M23" s="16"/>
@@ -3611,7 +4084,7 @@
         <v>549.53049999999996</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ref="D25:D29" si="4">$C$24/C25</f>
+        <f t="shared" ref="D25:D29" si="8">$C$24/C25</f>
         <v>1.9866592118180886</v>
       </c>
       <c r="F25" s="8">
@@ -3621,7 +4094,7 @@
         <v>3143.5584100000001</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" ref="H25:H29" si="5">$G$24/G25</f>
+        <f t="shared" ref="H25:H29" si="9">$G$24/G25</f>
         <v>1.9676495624587425</v>
       </c>
       <c r="J25" s="8">
@@ -3631,7 +4104,7 @@
         <v>2992.4668000000001</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" ref="L25:L29" si="6">$K$24/K25</f>
+        <f t="shared" ref="L25:L29" si="10">$K$24/K25</f>
         <v>1.9776768784870062</v>
       </c>
       <c r="N25" s="17"/>
@@ -3646,7 +4119,7 @@
         <v>278.34055000000001</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3.9222809252909787</v>
       </c>
       <c r="F26" s="8">
@@ -3656,7 +4129,7 @@
         <v>1558.1304399999999</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.9697711893748768</v>
       </c>
       <c r="J26" s="8">
@@ -3666,7 +4139,7 @@
         <v>1484.01116</v>
       </c>
       <c r="L26" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.9879298481825436</v>
       </c>
       <c r="N26" s="17"/>
@@ -3681,7 +4154,7 @@
         <v>140.59107</v>
       </c>
       <c r="D27" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.765285732586003</v>
       </c>
       <c r="F27" s="8">
@@ -3691,7 +4164,7 @@
         <v>790.47394999999995</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7.8249527767486846</v>
       </c>
       <c r="J27" s="8">
@@ -3701,7 +4174,7 @@
         <v>754.23893999999996</v>
       </c>
       <c r="L27" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7.8464954355180874</v>
       </c>
       <c r="N27" s="17"/>
@@ -3716,7 +4189,7 @@
         <v>72.71696</v>
       </c>
       <c r="D28" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>15.013414064614363</v>
       </c>
       <c r="F28" s="8">
@@ -3726,7 +4199,7 @@
         <v>406.64362</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15.210914485760284</v>
       </c>
       <c r="J28" s="8">
@@ -3736,7 +4209,7 @@
         <v>390.88560000000001</v>
       </c>
       <c r="L28" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>15.140318292615538</v>
       </c>
       <c r="N28" s="17"/>
@@ -3751,7 +4224,7 @@
         <v>40.928080000000001</v>
       </c>
       <c r="D29" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>26.674347538413723</v>
       </c>
       <c r="F29" s="11">
@@ -3761,7 +4234,7 @@
         <v>218.93725000000001</v>
       </c>
       <c r="H29" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>28.252028058267836</v>
       </c>
       <c r="J29" s="11">
@@ -3771,7 +4244,7 @@
         <v>210.65416999999999</v>
       </c>
       <c r="L29" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>28.094067162306832</v>
       </c>
       <c r="N29" s="17"/>
@@ -3780,16 +4253,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="N12:P12"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="N12:P12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3797,10 +4270,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593AA23E-9CFC-41E5-A923-4F16F489D36A}">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3811,820 +4284,840 @@
     <col min="4" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="25" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" customWidth="1"/>
+    <col min="18" max="25" width="8.7109375" customWidth="1"/>
     <col min="26" max="26" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="96" t="s">
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="42" t="s">
+      <c r="D2" s="151"/>
+      <c r="E2" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="48" t="s">
+      <c r="F2" s="153"/>
+      <c r="G2" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="54" t="s">
+      <c r="H2" s="155"/>
+      <c r="I2" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="90" t="s">
+      <c r="J2" s="157"/>
+      <c r="K2" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="91"/>
-      <c r="M2" s="66" t="s">
+      <c r="L2" s="147"/>
+      <c r="M2" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="67"/>
-      <c r="O2" s="72" t="s">
+      <c r="N2" s="149"/>
+      <c r="O2" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="78" t="s">
+      <c r="P2" s="139"/>
+      <c r="Q2" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="79"/>
-      <c r="S2" s="84" t="s">
+      <c r="R2" s="141"/>
+      <c r="S2" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="85"/>
-      <c r="U2" s="60" t="s">
+      <c r="T2" s="143"/>
+      <c r="U2" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="61"/>
-      <c r="W2" s="90" t="s">
+      <c r="V2" s="145"/>
+      <c r="W2" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="91"/>
-      <c r="Z2" s="140" t="s">
+      <c r="X2" s="147"/>
+      <c r="Z2" s="136" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="143"/>
-      <c r="B3" s="138" t="s">
+      <c r="A3" s="115"/>
+      <c r="B3" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="118" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="119" t="s">
+      <c r="D3" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="120" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="121" t="s">
+      <c r="F3" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="122" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="123" t="s">
+      <c r="H3" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="124" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="125" t="s">
+      <c r="J3" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="126" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="127" t="s">
+      <c r="L3" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="128" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="129" t="s">
+      <c r="N3" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="130" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="131" t="s">
+      <c r="P3" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="133" t="s">
+      <c r="R3" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="134" t="s">
-        <v>1</v>
-      </c>
-      <c r="U3" s="135" t="s">
+      <c r="T3" s="108" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="136" t="s">
-        <v>1</v>
-      </c>
-      <c r="W3" s="125" t="s">
+      <c r="V3" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="X3" s="126" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="141"/>
+      <c r="X3" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="137"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="137">
-        <v>1</v>
-      </c>
-      <c r="C4" s="98">
+      <c r="B4" s="111">
+        <v>1</v>
+      </c>
+      <c r="C4" s="72">
         <v>6344.3038299999998</v>
       </c>
-      <c r="D4" s="99">
+      <c r="D4" s="73">
         <f>$C$4/C4</f>
         <v>1</v>
       </c>
-      <c r="E4" s="100">
+      <c r="E4" s="74">
         <v>6109.1739200000002</v>
       </c>
-      <c r="F4" s="101">
+      <c r="F4" s="75">
         <f>$E$4/E4</f>
         <v>1</v>
       </c>
-      <c r="G4" s="102">
+      <c r="G4" s="76">
         <v>1238.5593100000001</v>
       </c>
-      <c r="H4" s="103">
+      <c r="H4" s="77">
         <f>$G$4/G4</f>
         <v>1</v>
       </c>
-      <c r="I4" s="104">
+      <c r="I4" s="78">
         <v>3805.0702200000001</v>
       </c>
-      <c r="J4" s="105">
+      <c r="J4" s="79">
         <f>$I$4/I4</f>
         <v>1</v>
       </c>
-      <c r="K4" s="106">
+      <c r="K4" s="80">
         <v>225.50916000000001</v>
       </c>
-      <c r="L4" s="107">
+      <c r="L4" s="81">
         <f>$K$4/K4</f>
         <v>1</v>
       </c>
-      <c r="M4" s="108">
+      <c r="M4" s="82">
         <v>1552.02189</v>
       </c>
-      <c r="N4" s="109">
+      <c r="N4" s="83">
         <f>$M$4/M4</f>
         <v>1</v>
       </c>
-      <c r="O4" s="110">
+      <c r="O4" s="84">
         <v>4992.0573599999998</v>
       </c>
-      <c r="P4" s="111">
+      <c r="P4" s="85">
         <f>$O$4/O4</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="112">
+      <c r="Q4" s="86">
         <v>1528.09917</v>
       </c>
-      <c r="R4" s="113">
+      <c r="R4" s="87">
         <f>$Q$4/Q4</f>
         <v>1</v>
       </c>
-      <c r="S4" s="114">
+      <c r="S4" s="88">
         <v>1091.72983</v>
       </c>
-      <c r="T4" s="115">
+      <c r="T4" s="89">
         <f>$S$4/S4</f>
         <v>1</v>
       </c>
-      <c r="U4" s="116">
+      <c r="U4" s="90">
         <v>6185.4213300000001</v>
       </c>
-      <c r="V4" s="117">
+      <c r="V4" s="91">
         <f>$U$4/U4</f>
         <v>1</v>
       </c>
-      <c r="W4" s="106">
+      <c r="W4" s="80">
         <v>5918.1324000000004</v>
       </c>
-      <c r="X4" s="107">
+      <c r="X4" s="81">
         <f>$W$4/W4</f>
         <v>1</v>
       </c>
-      <c r="Z4" s="142">
+      <c r="Z4" s="114">
         <f>AVERAGE(D4,F4,H4,J4,L4,N4,P4,R4,T4,V4,X4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="36">
+      <c r="B5" s="30">
         <v>2</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="32">
         <v>3211.6042600000001</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="33">
         <f t="shared" ref="D5:D9" si="0">$C$4/C5</f>
         <v>1.9754313783355113</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="36">
         <v>3009.9733200000001</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="37">
         <f t="shared" ref="F5:F9" si="1">$E$4/E5</f>
         <v>2.0296438773749661</v>
       </c>
-      <c r="G5" s="50">
+      <c r="G5" s="40">
         <v>635.85972000000004</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="41">
         <f t="shared" ref="H5:H9" si="2">$G$4/G5</f>
         <v>1.9478499282829238</v>
       </c>
-      <c r="I5" s="56">
+      <c r="I5" s="44">
         <v>1904.85754</v>
       </c>
-      <c r="J5" s="57">
+      <c r="J5" s="45">
         <f t="shared" ref="J5:J9" si="3">$I$4/I5</f>
         <v>1.997561570929866</v>
       </c>
-      <c r="K5" s="92">
+      <c r="K5" s="68">
         <v>113.95151</v>
       </c>
-      <c r="L5" s="93">
+      <c r="L5" s="69">
         <f t="shared" ref="L5:L9" si="4">$K$4/K5</f>
         <v>1.9789922924233301</v>
       </c>
-      <c r="M5" s="68">
+      <c r="M5" s="52">
         <v>782.59691999999995</v>
       </c>
-      <c r="N5" s="69">
+      <c r="N5" s="53">
         <f t="shared" ref="N5:N9" si="5">$M$4/M5</f>
         <v>1.9831689217483761</v>
       </c>
-      <c r="O5" s="74">
+      <c r="O5" s="56">
         <v>2489.4723800000002</v>
       </c>
-      <c r="P5" s="75">
+      <c r="P5" s="57">
         <f t="shared" ref="P5:P9" si="6">$O$4/O5</f>
         <v>2.0052672205184296</v>
       </c>
-      <c r="Q5" s="80">
+      <c r="Q5" s="60">
         <v>760.24554000000001</v>
       </c>
-      <c r="R5" s="81">
+      <c r="R5" s="61">
         <f t="shared" ref="R5:R9" si="7">$Q$4/Q5</f>
         <v>2.0100074115528517</v>
       </c>
-      <c r="S5" s="86">
+      <c r="S5" s="64">
         <v>549.53049999999996</v>
       </c>
-      <c r="T5" s="87">
+      <c r="T5" s="65">
         <f t="shared" ref="T5:T9" si="8">$S$4/S5</f>
         <v>1.9866592118180886</v>
       </c>
-      <c r="U5" s="62">
+      <c r="U5" s="48">
         <v>3143.5584100000001</v>
       </c>
-      <c r="V5" s="63">
+      <c r="V5" s="49">
         <f t="shared" ref="V5:V9" si="9">$U$4/U5</f>
         <v>1.9676495624587425</v>
       </c>
-      <c r="W5" s="92">
+      <c r="W5" s="68">
         <v>2992.4668000000001</v>
       </c>
-      <c r="X5" s="93">
+      <c r="X5" s="69">
         <f t="shared" ref="X5:X9" si="10">$W$4/W5</f>
         <v>1.9776768784870062</v>
       </c>
-      <c r="Z5" s="142">
+      <c r="Z5" s="114">
         <f t="shared" ref="Z5:Z9" si="11">AVERAGE(D5,F5,H5,J5,L5,N5,P5,R5,T5,V5,X5)</f>
         <v>1.9872643867209177</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="36">
+      <c r="B6" s="30">
         <v>4</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="32">
         <v>1581.87771</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="33">
         <f t="shared" si="0"/>
         <v>4.0106158585419349</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="36">
         <v>1535.1008899999999</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="37">
         <f t="shared" si="1"/>
         <v>3.9796562947729126</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="40">
         <v>312.61554000000001</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="41">
         <f t="shared" si="2"/>
         <v>3.9619249574093471</v>
       </c>
-      <c r="I6" s="56">
+      <c r="I6" s="44">
         <v>959.87148999999999</v>
       </c>
-      <c r="J6" s="57">
+      <c r="J6" s="45">
         <f t="shared" si="3"/>
         <v>3.9641454711817725</v>
       </c>
-      <c r="K6" s="92">
+      <c r="K6" s="68">
         <v>57.761960000000002</v>
       </c>
-      <c r="L6" s="93">
+      <c r="L6" s="69">
         <f t="shared" si="4"/>
         <v>3.9041119795796404</v>
       </c>
-      <c r="M6" s="68">
+      <c r="M6" s="52">
         <v>391.79863999999998</v>
       </c>
-      <c r="N6" s="69">
+      <c r="N6" s="53">
         <f t="shared" si="5"/>
         <v>3.9612743168276441</v>
       </c>
-      <c r="O6" s="74">
+      <c r="O6" s="56">
         <v>1251.8728799999999</v>
       </c>
-      <c r="P6" s="75">
+      <c r="P6" s="57">
         <f t="shared" si="6"/>
         <v>3.9876711443737003</v>
       </c>
-      <c r="Q6" s="80">
+      <c r="Q6" s="60">
         <v>384.14166</v>
       </c>
-      <c r="R6" s="81">
+      <c r="R6" s="61">
         <f t="shared" si="7"/>
         <v>3.977957428517386</v>
       </c>
-      <c r="S6" s="86">
+      <c r="S6" s="64">
         <v>278.34055000000001</v>
       </c>
-      <c r="T6" s="87">
+      <c r="T6" s="65">
         <f t="shared" si="8"/>
         <v>3.9222809252909787</v>
       </c>
-      <c r="U6" s="62">
+      <c r="U6" s="48">
         <v>1558.1304399999999</v>
       </c>
-      <c r="V6" s="63">
+      <c r="V6" s="49">
         <f t="shared" si="9"/>
         <v>3.9697711893748768</v>
       </c>
-      <c r="W6" s="92">
+      <c r="W6" s="68">
         <v>1484.01116</v>
       </c>
-      <c r="X6" s="93">
+      <c r="X6" s="69">
         <f t="shared" si="10"/>
         <v>3.9879298481825436</v>
       </c>
-      <c r="Z6" s="142">
+      <c r="Z6" s="114">
         <f t="shared" si="11"/>
         <v>3.9661217649138849</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="36">
+      <c r="B7" s="30">
         <v>8</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="32">
         <v>804.27999</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="33">
         <f t="shared" si="0"/>
         <v>7.8881781330901939</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="36">
         <v>763.15341000000001</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="37">
         <f t="shared" si="1"/>
         <v>8.0051714897008726</v>
       </c>
-      <c r="G7" s="50">
+      <c r="G7" s="40">
         <v>157.44566</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="41">
         <f t="shared" si="2"/>
         <v>7.8665827308291636</v>
       </c>
-      <c r="I7" s="56">
+      <c r="I7" s="44">
         <v>481.52929</v>
       </c>
-      <c r="J7" s="57">
+      <c r="J7" s="45">
         <f t="shared" si="3"/>
         <v>7.9020535178659639</v>
       </c>
-      <c r="K7" s="92">
+      <c r="K7" s="68">
         <v>29.097989999999999</v>
       </c>
-      <c r="L7" s="93">
+      <c r="L7" s="69">
         <f t="shared" si="4"/>
         <v>7.7499909787583272</v>
       </c>
-      <c r="M7" s="68">
+      <c r="M7" s="52">
         <v>198.25934000000001</v>
       </c>
-      <c r="N7" s="69">
+      <c r="N7" s="53">
         <f t="shared" si="5"/>
         <v>7.8282409797187862</v>
       </c>
-      <c r="O7" s="74">
+      <c r="O7" s="56">
         <v>637.38895000000002</v>
       </c>
-      <c r="P7" s="75">
+      <c r="P7" s="57">
         <f t="shared" si="6"/>
         <v>7.8320425228582948</v>
       </c>
-      <c r="Q7" s="80">
+      <c r="Q7" s="60">
         <v>193.59109000000001</v>
       </c>
-      <c r="R7" s="81">
+      <c r="R7" s="61">
         <f t="shared" si="7"/>
         <v>7.8934375027280437</v>
       </c>
-      <c r="S7" s="86">
+      <c r="S7" s="64">
         <v>140.59107</v>
       </c>
-      <c r="T7" s="87">
+      <c r="T7" s="65">
         <f t="shared" si="8"/>
         <v>7.765285732586003</v>
       </c>
-      <c r="U7" s="62">
+      <c r="U7" s="48">
         <v>790.47394999999995</v>
       </c>
-      <c r="V7" s="63">
+      <c r="V7" s="49">
         <f t="shared" si="9"/>
         <v>7.8249527767486846</v>
       </c>
-      <c r="W7" s="92">
+      <c r="W7" s="68">
         <v>754.23893999999996</v>
       </c>
-      <c r="X7" s="93">
+      <c r="X7" s="69">
         <f t="shared" si="10"/>
         <v>7.8464954355180874</v>
       </c>
-      <c r="Z7" s="142">
+      <c r="Z7" s="114">
         <f t="shared" si="11"/>
         <v>7.8547665273093115</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="36">
+      <c r="B8" s="30">
         <v>16</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="32">
         <v>416.85750000000002</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="33">
         <f t="shared" si="0"/>
         <v>15.219358725703627</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="36">
         <v>400.87011000000001</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="37">
         <f t="shared" si="1"/>
         <v>15.239784078688231</v>
       </c>
-      <c r="G8" s="50">
+      <c r="G8" s="40">
         <v>82.123540000000006</v>
       </c>
-      <c r="H8" s="51">
+      <c r="H8" s="41">
         <f t="shared" si="2"/>
         <v>15.081660020987892</v>
       </c>
-      <c r="I8" s="56">
+      <c r="I8" s="44">
         <v>252.37853000000001</v>
       </c>
-      <c r="J8" s="57">
+      <c r="J8" s="45">
         <f t="shared" si="3"/>
         <v>15.076838033726562</v>
       </c>
-      <c r="K8" s="92">
+      <c r="K8" s="68">
         <v>15.266859999999999</v>
       </c>
-      <c r="L8" s="93">
+      <c r="L8" s="69">
         <f t="shared" si="4"/>
         <v>14.771155299780048</v>
       </c>
-      <c r="M8" s="68">
+      <c r="M8" s="52">
         <v>104.86624</v>
       </c>
-      <c r="N8" s="69">
+      <c r="N8" s="53">
         <f t="shared" si="5"/>
         <v>14.80001466630252</v>
       </c>
-      <c r="O8" s="74">
+      <c r="O8" s="56">
         <v>330.64924000000002</v>
       </c>
-      <c r="P8" s="75">
+      <c r="P8" s="57">
         <f t="shared" si="6"/>
         <v>15.097743336715364</v>
       </c>
-      <c r="Q8" s="80">
+      <c r="Q8" s="60">
         <v>102.10281000000001</v>
       </c>
-      <c r="R8" s="81">
+      <c r="R8" s="61">
         <f t="shared" si="7"/>
         <v>14.966279282617196</v>
       </c>
-      <c r="S8" s="86">
+      <c r="S8" s="64">
         <v>72.71696</v>
       </c>
-      <c r="T8" s="87">
+      <c r="T8" s="65">
         <f t="shared" si="8"/>
         <v>15.013414064614363</v>
       </c>
-      <c r="U8" s="62">
+      <c r="U8" s="48">
         <v>406.64362</v>
       </c>
-      <c r="V8" s="63">
+      <c r="V8" s="49">
         <f t="shared" si="9"/>
         <v>15.210914485760284</v>
       </c>
-      <c r="W8" s="92">
+      <c r="W8" s="68">
         <v>390.88560000000001</v>
       </c>
-      <c r="X8" s="93">
+      <c r="X8" s="69">
         <f t="shared" si="10"/>
         <v>15.140318292615538</v>
       </c>
-      <c r="Z8" s="142">
+      <c r="Z8" s="114">
         <f t="shared" si="11"/>
         <v>15.056134571591963</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="37">
+      <c r="B9" s="31">
         <v>32</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="34">
         <v>227.58150000000001</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="35">
         <f t="shared" si="0"/>
         <v>27.877063074107514</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="38">
         <v>214.18790000000001</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="39">
         <f t="shared" si="1"/>
         <v>28.522497862857797</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="42">
         <v>45.179659999999998</v>
       </c>
-      <c r="H9" s="53">
+      <c r="H9" s="43">
         <f t="shared" si="2"/>
         <v>27.414090986961835</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="46">
         <v>135.40665999999999</v>
       </c>
-      <c r="J9" s="59">
+      <c r="J9" s="47">
         <f t="shared" si="3"/>
         <v>28.101056624541219</v>
       </c>
-      <c r="K9" s="94">
+      <c r="K9" s="70">
         <v>9.0215899999999998</v>
       </c>
-      <c r="L9" s="95">
+      <c r="L9" s="71">
         <f t="shared" si="4"/>
         <v>24.996609245155234</v>
       </c>
-      <c r="M9" s="70">
+      <c r="M9" s="54">
         <v>56.578319999999998</v>
       </c>
-      <c r="N9" s="71">
+      <c r="N9" s="55">
         <f t="shared" si="5"/>
         <v>27.431388736887204</v>
       </c>
-      <c r="O9" s="76">
+      <c r="O9" s="58">
         <v>181.62129999999999</v>
       </c>
-      <c r="P9" s="77">
+      <c r="P9" s="59">
         <f t="shared" si="6"/>
         <v>27.486078780407365</v>
       </c>
-      <c r="Q9" s="82">
+      <c r="Q9" s="62">
         <v>54.212049999999998</v>
       </c>
-      <c r="R9" s="83">
+      <c r="R9" s="63">
         <f t="shared" si="7"/>
         <v>28.187444857739195</v>
       </c>
-      <c r="S9" s="88">
+      <c r="S9" s="66">
         <v>40.928080000000001</v>
       </c>
-      <c r="T9" s="89">
+      <c r="T9" s="67">
         <f t="shared" si="8"/>
         <v>26.674347538413723</v>
       </c>
-      <c r="U9" s="64">
+      <c r="U9" s="50">
         <v>218.93725000000001</v>
       </c>
-      <c r="V9" s="65">
+      <c r="V9" s="51">
         <f t="shared" si="9"/>
         <v>28.252028058267836</v>
       </c>
-      <c r="W9" s="94">
+      <c r="W9" s="70">
         <v>210.65416999999999</v>
       </c>
-      <c r="X9" s="95">
+      <c r="X9" s="71">
         <f t="shared" si="10"/>
         <v>28.094067162306832</v>
       </c>
-      <c r="Z9" s="142">
+      <c r="Z9" s="114">
         <f t="shared" si="11"/>
         <v>27.548788447967794</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="148"/>
-      <c r="C12" s="149" t="s">
+      <c r="B12" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="149" t="s">
+      <c r="D12" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="149" t="s">
+      <c r="E12" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="149" t="s">
+      <c r="F12" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="149" t="s">
+      <c r="G12" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="149" t="s">
+      <c r="H12" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="149" t="s">
+      <c r="I12" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="149" t="s">
+      <c r="J12" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="149" t="s">
+      <c r="K12" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="149" t="s">
+      <c r="L12" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="150" t="s">
+      <c r="M12" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="O12" s="139"/>
-      <c r="P12" s="156" t="s">
+      <c r="O12" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="158" t="s">
         <v>26</v>
       </c>
+      <c r="Q12" s="128" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="146">
+      <c r="C13" s="118">
         <v>0</v>
       </c>
-      <c r="D13" s="145">
+      <c r="D13" s="117">
         <v>3.708501</v>
       </c>
-      <c r="E13" s="145">
+      <c r="E13" s="117">
         <v>11.017976000000001</v>
       </c>
-      <c r="F13" s="145">
+      <c r="F13" s="117">
         <v>15.069315</v>
       </c>
-      <c r="G13" s="145">
+      <c r="G13" s="117">
         <v>8.8101599999999998</v>
       </c>
-      <c r="H13" s="145">
+      <c r="H13" s="117">
         <v>15.717249000000001</v>
       </c>
-      <c r="I13" s="145">
+      <c r="I13" s="117">
         <v>7.9499180000000003</v>
       </c>
-      <c r="J13" s="147">
+      <c r="J13" s="119">
         <v>3.113645</v>
       </c>
-      <c r="K13" s="145">
+      <c r="K13" s="117">
         <v>9.0983169999999998</v>
       </c>
-      <c r="L13" s="145">
+      <c r="L13" s="117">
         <v>12.853278</v>
       </c>
-      <c r="M13" s="151">
+      <c r="M13" s="123">
         <v>15.432489</v>
       </c>
-      <c r="O13" s="157" t="s">
+      <c r="O13" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="P13" s="158">
+      <c r="P13" s="162">
         <v>9478</v>
       </c>
+      <c r="Q13" s="159" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="147">
+      <c r="C14" s="119">
         <v>3.708501</v>
       </c>
-      <c r="D14" s="146">
+      <c r="D14" s="118">
         <v>0</v>
       </c>
-      <c r="E14" s="145">
+      <c r="E14" s="117">
         <v>14.143967999999999</v>
       </c>
-      <c r="F14" s="145">
+      <c r="F14" s="117">
         <v>11.963168</v>
       </c>
-      <c r="G14" s="145">
+      <c r="G14" s="117">
         <v>7.348312</v>
       </c>
-      <c r="H14" s="145">
+      <c r="H14" s="117">
         <v>18.627376999999999</v>
       </c>
-      <c r="I14" s="145">
+      <c r="I14" s="117">
         <v>10.534774000000001</v>
       </c>
-      <c r="J14" s="145">
+      <c r="J14" s="117">
         <v>6.1968019999999999</v>
       </c>
-      <c r="K14" s="145">
+      <c r="K14" s="117">
         <v>9.5868249999999993</v>
       </c>
-      <c r="L14" s="145">
+      <c r="L14" s="117">
         <v>13.231009999999999</v>
       </c>
-      <c r="M14" s="151">
+      <c r="M14" s="123">
         <v>18.51323</v>
       </c>
-      <c r="O14" s="157" t="s">
+      <c r="O14" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="P14" s="158">
+      <c r="P14" s="162">
         <v>1687</v>
       </c>
+      <c r="Q14" s="160" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="145">
+      <c r="C15" s="117">
         <v>11.017976000000001</v>
       </c>
-      <c r="D15" s="145">
+      <c r="D15" s="117">
         <v>14.143967999999999</v>
       </c>
-      <c r="E15" s="146">
+      <c r="E15" s="118">
         <v>0</v>
       </c>
-      <c r="F15" s="145">
+      <c r="F15" s="117">
         <v>26.085691000000001</v>
       </c>
-      <c r="G15" s="145">
+      <c r="G15" s="117">
         <v>16.468078999999999</v>
       </c>
-      <c r="H15" s="145">
+      <c r="H15" s="117">
         <v>6.7052069999999997</v>
       </c>
-      <c r="I15" s="145">
+      <c r="I15" s="117">
         <v>7.9040299999999997</v>
       </c>
-      <c r="J15" s="145">
+      <c r="J15" s="117">
         <v>8.064584</v>
       </c>
-      <c r="K15" s="145">
+      <c r="K15" s="117">
         <v>13.836762999999999</v>
       </c>
-      <c r="L15" s="145">
+      <c r="L15" s="117">
         <v>16.402566</v>
       </c>
-      <c r="M15" s="152">
+      <c r="M15" s="124">
         <v>4.4361519999999999</v>
       </c>
-      <c r="O15" s="157" t="s">
+      <c r="O15" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="P15" s="158">
+      <c r="P15" s="162">
         <v>5538</v>
+      </c>
+      <c r="Q15" s="161" t="s">
+        <v>32</v>
       </c>
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
@@ -4634,47 +5127,50 @@
       <c r="AB15" s="15"/>
     </row>
     <row r="16" spans="1:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="145">
+      <c r="C16" s="117">
         <v>15.069315</v>
       </c>
-      <c r="D16" s="147">
+      <c r="D16" s="119">
         <v>11.963168</v>
       </c>
-      <c r="E16" s="145">
+      <c r="E16" s="117">
         <v>26.085691000000001</v>
       </c>
-      <c r="F16" s="146">
+      <c r="F16" s="118">
         <v>0</v>
       </c>
-      <c r="G16" s="145">
+      <c r="G16" s="117">
         <v>13.412691000000001</v>
       </c>
-      <c r="H16" s="145">
+      <c r="H16" s="117">
         <v>30.326366</v>
       </c>
-      <c r="I16" s="145">
+      <c r="I16" s="117">
         <v>21.746663999999999</v>
       </c>
-      <c r="J16" s="145">
+      <c r="J16" s="117">
         <v>18.150805999999999</v>
       </c>
-      <c r="K16" s="145">
+      <c r="K16" s="117">
         <v>18.257642000000001</v>
       </c>
-      <c r="L16" s="145">
+      <c r="L16" s="117">
         <v>20.360185000000001</v>
       </c>
-      <c r="M16" s="151">
+      <c r="M16" s="123">
         <v>30.473040999999998</v>
       </c>
-      <c r="O16" s="157" t="s">
+      <c r="O16" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="P16" s="158">
+      <c r="P16" s="162">
         <v>301</v>
+      </c>
+      <c r="Q16" s="161" t="s">
+        <v>33</v>
       </c>
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
@@ -4684,47 +5180,50 @@
       <c r="AB16" s="15"/>
     </row>
     <row r="17" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="145">
+      <c r="C17" s="117">
         <v>8.8101599999999998</v>
       </c>
-      <c r="D17" s="147">
+      <c r="D17" s="119">
         <v>7.348312</v>
       </c>
-      <c r="E17" s="145">
+      <c r="E17" s="117">
         <v>16.468078999999999</v>
       </c>
-      <c r="F17" s="145">
+      <c r="F17" s="117">
         <v>13.412691000000001</v>
       </c>
-      <c r="G17" s="146">
+      <c r="G17" s="118">
         <v>0</v>
       </c>
-      <c r="H17" s="145">
+      <c r="H17" s="117">
         <v>19.365057</v>
       </c>
-      <c r="I17" s="145">
+      <c r="I17" s="117">
         <v>15.565144</v>
       </c>
-      <c r="J17" s="145">
+      <c r="J17" s="117">
         <v>10.072918</v>
       </c>
-      <c r="K17" s="145">
+      <c r="K17" s="117">
         <v>15.235410999999999</v>
       </c>
-      <c r="L17" s="145">
+      <c r="L17" s="117">
         <v>18.560316</v>
       </c>
-      <c r="M17" s="151">
+      <c r="M17" s="123">
         <v>19.901475000000001</v>
       </c>
-      <c r="O17" s="157" t="s">
+      <c r="O17" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="P17" s="158">
+      <c r="P17" s="162">
         <v>2135</v>
+      </c>
+      <c r="Q17" s="161" t="s">
+        <v>34</v>
       </c>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
@@ -4734,47 +5233,50 @@
       <c r="AB17" s="15"/>
     </row>
     <row r="18" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="145">
+      <c r="C18" s="117">
         <v>15.717249000000001</v>
       </c>
-      <c r="D18" s="145">
+      <c r="D18" s="117">
         <v>18.627376999999999</v>
       </c>
-      <c r="E18" s="145">
+      <c r="E18" s="117">
         <v>6.7052069999999997</v>
       </c>
-      <c r="F18" s="145">
+      <c r="F18" s="117">
         <v>30.326366</v>
       </c>
-      <c r="G18" s="145">
+      <c r="G18" s="117">
         <v>19.365057</v>
       </c>
-      <c r="H18" s="146">
+      <c r="H18" s="118">
         <v>0</v>
       </c>
-      <c r="I18" s="145">
+      <c r="I18" s="117">
         <v>14.009862999999999</v>
       </c>
-      <c r="J18" s="145">
+      <c r="J18" s="117">
         <v>12.783825999999999</v>
       </c>
-      <c r="K18" s="145">
+      <c r="K18" s="117">
         <v>19.916284000000001</v>
       </c>
-      <c r="L18" s="145">
+      <c r="L18" s="117">
         <v>22.812947999999999</v>
       </c>
-      <c r="M18" s="152">
+      <c r="M18" s="124">
         <v>5.7946759999999999</v>
       </c>
-      <c r="O18" s="157" t="s">
+      <c r="O18" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="P18" s="158">
+      <c r="P18" s="162">
         <v>7573</v>
+      </c>
+      <c r="Q18" s="161" t="s">
+        <v>35</v>
       </c>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
@@ -4784,47 +5286,50 @@
       <c r="AB18" s="15"/>
     </row>
     <row r="19" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="145">
+      <c r="C19" s="117">
         <v>7.9499180000000003</v>
       </c>
-      <c r="D19" s="145">
+      <c r="D19" s="117">
         <v>10.534774000000001</v>
       </c>
-      <c r="E19" s="145">
+      <c r="E19" s="117">
         <v>7.9040299999999997</v>
       </c>
-      <c r="F19" s="145">
+      <c r="F19" s="117">
         <v>21.746663999999999</v>
       </c>
-      <c r="G19" s="145">
+      <c r="G19" s="117">
         <v>15.565144</v>
       </c>
-      <c r="H19" s="145">
+      <c r="H19" s="117">
         <v>14.009862999999999</v>
       </c>
-      <c r="I19" s="146">
+      <c r="I19" s="118">
         <v>0</v>
       </c>
-      <c r="J19" s="147">
+      <c r="J19" s="119">
         <v>6.5823450000000001</v>
       </c>
-      <c r="K19" s="145">
+      <c r="K19" s="117">
         <v>6.7725020000000002</v>
       </c>
-      <c r="L19" s="145">
+      <c r="L19" s="117">
         <v>8.9502500000000005</v>
       </c>
-      <c r="M19" s="151">
+      <c r="M19" s="123">
         <v>10.982179</v>
       </c>
-      <c r="O19" s="157" t="s">
+      <c r="O19" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="P19" s="158">
+      <c r="P19" s="162">
         <v>2087</v>
+      </c>
+      <c r="Q19" s="161" t="s">
+        <v>36</v>
       </c>
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
@@ -4834,47 +5339,50 @@
       <c r="AB19" s="15"/>
     </row>
     <row r="20" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="147">
+      <c r="C20" s="119">
         <v>3.113645</v>
       </c>
-      <c r="D20" s="145">
+      <c r="D20" s="117">
         <v>6.1968019999999999</v>
       </c>
-      <c r="E20" s="145">
+      <c r="E20" s="117">
         <v>8.064584</v>
       </c>
-      <c r="F20" s="145">
+      <c r="F20" s="117">
         <v>18.150805999999999</v>
       </c>
-      <c r="G20" s="145">
+      <c r="G20" s="117">
         <v>10.072918</v>
       </c>
-      <c r="H20" s="145">
+      <c r="H20" s="117">
         <v>12.783825999999999</v>
       </c>
-      <c r="I20" s="145">
+      <c r="I20" s="117">
         <v>6.5823450000000001</v>
       </c>
-      <c r="J20" s="146">
+      <c r="J20" s="118">
         <v>0</v>
       </c>
-      <c r="K20" s="145">
+      <c r="K20" s="117">
         <v>9.5082850000000008</v>
       </c>
-      <c r="L20" s="145">
+      <c r="L20" s="117">
         <v>13.17277</v>
       </c>
-      <c r="M20" s="151">
+      <c r="M20" s="123">
         <v>12.330344</v>
       </c>
-      <c r="O20" s="157" t="s">
+      <c r="O20" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="P20" s="158">
+      <c r="P20" s="162">
         <v>1480</v>
+      </c>
+      <c r="Q20" s="161" t="s">
+        <v>37</v>
       </c>
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
@@ -4884,47 +5392,50 @@
       <c r="AB20" s="15"/>
     </row>
     <row r="21" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="145">
+      <c r="C21" s="117">
         <v>9.0983169999999998</v>
       </c>
-      <c r="D21" s="145">
+      <c r="D21" s="117">
         <v>9.5868249999999993</v>
       </c>
-      <c r="E21" s="145">
+      <c r="E21" s="117">
         <v>13.836762999999999</v>
       </c>
-      <c r="F21" s="145">
+      <c r="F21" s="117">
         <v>18.257642000000001</v>
       </c>
-      <c r="G21" s="145">
+      <c r="G21" s="117">
         <v>15.235410999999999</v>
       </c>
-      <c r="H21" s="145">
+      <c r="H21" s="117">
         <v>19.916284000000001</v>
       </c>
-      <c r="I21" s="145">
+      <c r="I21" s="117">
         <v>6.7725020000000002</v>
       </c>
-      <c r="J21" s="145">
+      <c r="J21" s="117">
         <v>9.5082850000000008</v>
       </c>
-      <c r="K21" s="146">
+      <c r="K21" s="118">
         <v>0</v>
       </c>
-      <c r="L21" s="147">
+      <c r="L21" s="119">
         <v>3.893904</v>
       </c>
-      <c r="M21" s="151">
+      <c r="M21" s="123">
         <v>16.919685999999999</v>
       </c>
-      <c r="O21" s="157" t="s">
+      <c r="O21" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="P21" s="158">
+      <c r="P21" s="162">
         <v>9757</v>
+      </c>
+      <c r="Q21" s="160" t="s">
+        <v>38</v>
       </c>
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
@@ -4934,47 +5445,50 @@
       <c r="AB21" s="15"/>
     </row>
     <row r="22" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="145">
+      <c r="C22" s="117">
         <v>12.853278</v>
       </c>
-      <c r="D22" s="145">
+      <c r="D22" s="117">
         <v>13.231009999999999</v>
       </c>
-      <c r="E22" s="145">
+      <c r="E22" s="117">
         <v>16.402566</v>
       </c>
-      <c r="F22" s="145">
+      <c r="F22" s="117">
         <v>20.360185000000001</v>
       </c>
-      <c r="G22" s="145">
+      <c r="G22" s="117">
         <v>18.560316</v>
       </c>
-      <c r="H22" s="145">
+      <c r="H22" s="117">
         <v>22.812947999999999</v>
       </c>
-      <c r="I22" s="145">
+      <c r="I22" s="117">
         <v>8.9502500000000005</v>
       </c>
-      <c r="J22" s="145">
+      <c r="J22" s="117">
         <v>13.17277</v>
       </c>
-      <c r="K22" s="147">
+      <c r="K22" s="119">
         <v>3.893904</v>
       </c>
-      <c r="L22" s="146">
+      <c r="L22" s="118">
         <v>0</v>
       </c>
-      <c r="M22" s="151">
+      <c r="M22" s="123">
         <v>19.180605</v>
       </c>
-      <c r="O22" s="157" t="s">
+      <c r="O22" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="P22" s="158">
+      <c r="P22" s="162">
         <v>9239</v>
+      </c>
+      <c r="Q22" s="161" t="s">
+        <v>39</v>
       </c>
       <c r="W22" s="15"/>
       <c r="X22" s="15"/>
@@ -4984,47 +5498,50 @@
       <c r="AB22" s="15"/>
     </row>
     <row r="23" spans="2:28" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="153">
+      <c r="C23" s="125">
         <v>15.432489</v>
       </c>
-      <c r="D23" s="153">
+      <c r="D23" s="125">
         <v>18.51323</v>
       </c>
-      <c r="E23" s="154">
+      <c r="E23" s="126">
         <v>4.4361519999999999</v>
       </c>
-      <c r="F23" s="153">
+      <c r="F23" s="125">
         <v>30.473040999999998</v>
       </c>
-      <c r="G23" s="153">
+      <c r="G23" s="125">
         <v>19.901475000000001</v>
       </c>
-      <c r="H23" s="153">
+      <c r="H23" s="125">
         <v>5.7946759999999999</v>
       </c>
-      <c r="I23" s="153">
+      <c r="I23" s="125">
         <v>10.982179</v>
       </c>
-      <c r="J23" s="153">
+      <c r="J23" s="125">
         <v>12.330344</v>
       </c>
-      <c r="K23" s="153">
+      <c r="K23" s="125">
         <v>16.919685999999999</v>
       </c>
-      <c r="L23" s="153">
+      <c r="L23" s="125">
         <v>19.180605</v>
       </c>
-      <c r="M23" s="155">
+      <c r="M23" s="127">
         <v>0</v>
       </c>
-      <c r="O23" s="157" t="s">
+      <c r="O23" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="P23" s="158">
+      <c r="P23" s="162">
         <v>10050</v>
+      </c>
+      <c r="Q23" s="159" t="s">
+        <v>40</v>
       </c>
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
@@ -5049,20 +5566,104 @@
       <c r="AA25" s="15"/>
       <c r="AB25" s="15"/>
     </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C26" s="163">
+        <f>SUM(C4,E4,G4,I4,K4,M4,O4,Q4,S4,U4,W4)</f>
+        <v>38990.078420000005</v>
+      </c>
+      <c r="D26" s="164">
+        <f>$C$26/$C26</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="164">
+        <f>D26/B4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C27" s="163">
+        <f>SUM(C5,E5,G5,I5,K5,M5,O5,Q5,S5,U5,W5)</f>
+        <v>19594.116900000001</v>
+      </c>
+      <c r="D27" s="164">
+        <f>$C$26/$C27</f>
+        <v>1.9898869961319872</v>
+      </c>
+      <c r="E27" s="164">
+        <f t="shared" ref="E27:E31" si="12">D27/B5</f>
+        <v>0.99494349806599358</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C28" s="163">
+        <f>SUM(C6,E6,G6,I6,K6,M6,O6,Q6,S6,U6,W6)</f>
+        <v>9795.5229200000012</v>
+      </c>
+      <c r="D28" s="164">
+        <f t="shared" ref="D27:D31" si="13">$C$26/$C28</f>
+        <v>3.9803978550641785</v>
+      </c>
+      <c r="E28" s="164">
+        <f t="shared" si="12"/>
+        <v>0.99509946376604463</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C29" s="163">
+        <f>SUM(C7,E7,G7,I7,K7,M7,O7,Q7,S7,U7,W7)</f>
+        <v>4950.0496800000001</v>
+      </c>
+      <c r="D29" s="164">
+        <f t="shared" si="13"/>
+        <v>7.8767044657216463</v>
+      </c>
+      <c r="E29" s="164">
+        <f t="shared" si="12"/>
+        <v>0.98458805821520579</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C30" s="163">
+        <f>SUM(C8,E8,G8,I8,K8,M8,O8,Q8,S8,U8,W8)</f>
+        <v>2575.3610100000001</v>
+      </c>
+      <c r="D30" s="164">
+        <f t="shared" si="13"/>
+        <v>15.139655476883998</v>
+      </c>
+      <c r="E30" s="164">
+        <f t="shared" si="12"/>
+        <v>0.9462284673052499</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C31" s="163">
+        <f>SUM(C9,E9,G9,I9,K9,M9,O9,Q9,S9,U9,W9)</f>
+        <v>1394.3084799999999</v>
+      </c>
+      <c r="D31" s="164">
+        <f t="shared" si="13"/>
+        <v>27.963738999851746</v>
+      </c>
+      <c r="E31" s="164">
+        <f t="shared" si="12"/>
+        <v>0.87386684374536705</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="Z2:Z3"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>